<commit_message>
added alphanumeric types of input for form builder
</commit_message>
<xml_diff>
--- a/Authentication.WEB/ExcelConfig/config_file.xlsx
+++ b/Authentication.WEB/ExcelConfig/config_file.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="93">
   <si>
     <t>Field_ID</t>
   </si>
@@ -170,12 +170,6 @@
     <t>CC range</t>
   </si>
   <si>
-    <t>Number of seats</t>
-  </si>
-  <si>
-    <t>Make</t>
-  </si>
-  <si>
     <t>cc_range</t>
   </si>
   <si>
@@ -230,9 +224,6 @@
     <t>Тип на осигурителна ставка</t>
   </si>
   <si>
-    <t>is_alphanumeric</t>
-  </si>
-  <si>
     <t>Required</t>
   </si>
   <si>
@@ -242,12 +233,6 @@
     <t>number</t>
   </si>
   <si>
-    <t>alphanumeric</t>
-  </si>
-  <si>
-    <t>ne e napraveno</t>
-  </si>
-  <si>
     <t>Insured_Item_Type</t>
   </si>
   <si>
@@ -282,6 +267,45 @@
   </si>
   <si>
     <t>margin-left: -10%;</t>
+  </si>
+  <si>
+    <t>One</t>
+  </si>
+  <si>
+    <t>Two</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>two</t>
+  </si>
+  <si>
+    <t>One seat</t>
+  </si>
+  <si>
+    <t>Two seats</t>
+  </si>
+  <si>
+    <t>Submit</t>
+  </si>
+  <si>
+    <t>submit</t>
+  </si>
+  <si>
+    <t>dropdown;</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>alphanumericspacetextbox</t>
+  </si>
+  <si>
+    <t>alphanumerictextbox</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
@@ -352,106 +376,29 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color auto="1"/>
@@ -795,7 +742,7 @@
   <dimension ref="A1:Q21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:K16"/>
+      <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -822,40 +769,35 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>68</v>
-      </c>
       <c r="G1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" s="4"/>
-      <c r="N1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="O1" s="4"/>
+      <c r="J1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>78</v>
+      </c>
       <c r="Q1" s="2"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
@@ -863,28 +805,28 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>69</v>
+      </c>
+      <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>25</v>
+      <c r="D2">
+        <v>0</v>
       </c>
       <c r="E2" t="s">
         <v>25</v>
       </c>
-      <c r="F2">
-        <v>0</v>
+      <c r="F2" t="s">
+        <v>25</v>
       </c>
       <c r="G2">
         <v>0</v>
       </c>
-      <c r="I2" t="s">
-        <v>81</v>
-      </c>
-      <c r="K2" t="s">
-        <v>74</v>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="J2" t="s">
+        <v>76</v>
       </c>
       <c r="Q2" s="3"/>
     </row>
@@ -893,28 +835,28 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" t="s">
         <v>8</v>
       </c>
-      <c r="C3">
-        <v>0</v>
-      </c>
-      <c r="D3" t="s">
-        <v>25</v>
+      <c r="D3">
+        <v>0</v>
       </c>
       <c r="E3" t="s">
         <v>25</v>
       </c>
-      <c r="F3">
-        <v>0</v>
+      <c r="F3" t="s">
+        <v>25</v>
       </c>
       <c r="G3">
         <v>0</v>
       </c>
-      <c r="I3" t="s">
-        <v>81</v>
-      </c>
-      <c r="K3" t="s">
-        <v>17</v>
+      <c r="H3">
+        <v>0</v>
+      </c>
+      <c r="J3" t="s">
+        <v>76</v>
       </c>
       <c r="Q3" s="3"/>
     </row>
@@ -923,28 +865,28 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>25</v>
+        <v>68</v>
+      </c>
+      <c r="C4" t="s">
+        <v>66</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
       </c>
       <c r="E4" t="s">
         <v>25</v>
       </c>
-      <c r="F4">
-        <v>0</v>
+      <c r="F4" t="s">
+        <v>25</v>
       </c>
       <c r="G4">
         <v>0</v>
       </c>
-      <c r="I4" t="s">
-        <v>81</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>73</v>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="J4" t="s">
+        <v>76</v>
       </c>
       <c r="Q4" s="3"/>
     </row>
@@ -953,28 +895,28 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
+      <c r="D5">
+        <v>0</v>
       </c>
       <c r="E5" t="s">
         <v>25</v>
       </c>
-      <c r="F5">
-        <v>0</v>
+      <c r="F5" t="s">
+        <v>25</v>
       </c>
       <c r="G5">
         <v>0</v>
       </c>
-      <c r="I5" t="s">
-        <v>81</v>
-      </c>
-      <c r="K5" s="3" t="s">
-        <v>30</v>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="J5" t="s">
+        <v>76</v>
       </c>
       <c r="Q5" s="3"/>
     </row>
@@ -982,32 +924,32 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" t="s">
         <v>16</v>
       </c>
-      <c r="C6">
-        <v>0</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
+      <c r="D6">
+        <v>0</v>
       </c>
       <c r="E6" t="s">
         <v>25</v>
       </c>
-      <c r="F6">
-        <v>1</v>
+      <c r="F6" t="s">
+        <v>25</v>
       </c>
       <c r="G6">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6">
+        <v>0</v>
+      </c>
+      <c r="I6">
         <v>20</v>
       </c>
-      <c r="I6" t="s">
-        <v>81</v>
-      </c>
-      <c r="K6" s="5" t="s">
-        <v>77</v>
+      <c r="J6" t="s">
+        <v>76</v>
       </c>
       <c r="Q6" s="3"/>
     </row>
@@ -1016,28 +958,28 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" t="s">
         <v>8</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7" t="s">
-        <v>25</v>
+      <c r="D7">
+        <v>0</v>
       </c>
       <c r="E7" t="s">
         <v>25</v>
       </c>
-      <c r="F7">
-        <v>0</v>
+      <c r="F7" t="s">
+        <v>25</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
-      <c r="I7" t="s">
-        <v>81</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>46</v>
+      <c r="H7">
+        <v>0</v>
+      </c>
+      <c r="J7" t="s">
+        <v>76</v>
       </c>
       <c r="Q7" s="3"/>
     </row>
@@ -1046,28 +988,28 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
         <v>29</v>
       </c>
-      <c r="C8">
+      <c r="D8">
         <v>5</v>
       </c>
-      <c r="D8" t="s">
-        <v>25</v>
-      </c>
       <c r="E8" t="s">
         <v>25</v>
       </c>
-      <c r="F8">
-        <v>0</v>
+      <c r="F8" t="s">
+        <v>25</v>
       </c>
       <c r="G8">
         <v>0</v>
       </c>
-      <c r="I8" t="s">
-        <v>81</v>
-      </c>
-      <c r="K8" t="s">
-        <v>49</v>
+      <c r="H8">
+        <v>0</v>
+      </c>
+      <c r="J8" t="s">
+        <v>76</v>
       </c>
       <c r="Q8" s="3"/>
     </row>
@@ -1076,28 +1018,28 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" t="s">
         <v>8</v>
       </c>
-      <c r="C9">
-        <v>0</v>
-      </c>
-      <c r="D9" t="s">
-        <v>25</v>
+      <c r="D9">
+        <v>0</v>
       </c>
       <c r="E9" t="s">
         <v>25</v>
       </c>
-      <c r="F9">
-        <v>0</v>
+      <c r="F9" t="s">
+        <v>25</v>
       </c>
       <c r="G9">
         <v>0</v>
       </c>
-      <c r="I9" t="s">
-        <v>81</v>
-      </c>
-      <c r="K9" s="3" t="s">
-        <v>48</v>
+      <c r="H9">
+        <v>0</v>
+      </c>
+      <c r="J9" t="s">
+        <v>76</v>
       </c>
       <c r="Q9" s="3"/>
     </row>
@@ -1106,31 +1048,31 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>73</v>
+      </c>
+      <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
-        <v>25</v>
+      <c r="D10">
+        <v>0</v>
       </c>
       <c r="E10" t="s">
         <v>25</v>
       </c>
-      <c r="F10">
-        <v>0</v>
+      <c r="F10" t="s">
+        <v>82</v>
       </c>
       <c r="G10">
         <v>0</v>
       </c>
-      <c r="I10" t="s">
-        <v>81</v>
+      <c r="H10">
+        <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="K10" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="Q10" s="3"/>
     </row>
@@ -1139,28 +1081,28 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" t="s">
         <v>8</v>
       </c>
-      <c r="C11">
-        <v>0</v>
-      </c>
-      <c r="D11" t="s">
-        <v>25</v>
+      <c r="D11">
+        <v>0</v>
       </c>
       <c r="E11" t="s">
         <v>25</v>
       </c>
-      <c r="F11">
-        <v>0</v>
+      <c r="F11" t="s">
+        <v>25</v>
       </c>
       <c r="G11">
         <v>0</v>
       </c>
-      <c r="I11" t="s">
-        <v>81</v>
-      </c>
-      <c r="K11" s="3" t="s">
-        <v>47</v>
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="J11" t="s">
+        <v>76</v>
       </c>
       <c r="Q11" s="3"/>
     </row>
@@ -1169,30 +1111,30 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12" t="s">
-        <v>25</v>
+        <v>73</v>
+      </c>
+      <c r="C12" t="s">
+        <v>11</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
       </c>
       <c r="E12" t="s">
         <v>25</v>
       </c>
-      <c r="F12">
-        <v>0</v>
+      <c r="F12" t="s">
+        <v>83</v>
       </c>
       <c r="G12">
         <v>0</v>
       </c>
-      <c r="I12" t="s">
-        <v>81</v>
+      <c r="H12">
+        <v>0</v>
       </c>
       <c r="J12" t="s">
-        <v>84</v>
-      </c>
-      <c r="K12" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="K12" t="s">
         <v>79</v>
       </c>
       <c r="Q12" s="3"/>
@@ -1202,28 +1144,28 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>84</v>
+      </c>
+      <c r="C13" t="s">
         <v>8</v>
       </c>
-      <c r="C13">
-        <v>0</v>
-      </c>
-      <c r="D13" t="s">
-        <v>25</v>
+      <c r="D13">
+        <v>0</v>
       </c>
       <c r="E13" t="s">
         <v>25</v>
       </c>
-      <c r="F13">
-        <v>0</v>
+      <c r="F13" t="s">
+        <v>25</v>
       </c>
       <c r="G13">
         <v>0</v>
       </c>
-      <c r="I13" t="s">
-        <v>81</v>
-      </c>
-      <c r="K13" s="3" t="s">
-        <v>32</v>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="J13" t="s">
+        <v>76</v>
       </c>
       <c r="Q13" s="3"/>
     </row>
@@ -1232,28 +1174,31 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14">
-        <v>0</v>
-      </c>
-      <c r="D14" t="s">
-        <v>25</v>
+        <v>74</v>
+      </c>
+      <c r="C14" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
       </c>
       <c r="E14" t="s">
         <v>25</v>
       </c>
-      <c r="F14">
-        <v>1</v>
+      <c r="F14" t="s">
+        <v>82</v>
       </c>
       <c r="G14">
         <v>0</v>
       </c>
-      <c r="I14" t="s">
-        <v>81</v>
-      </c>
-      <c r="K14" s="3" t="s">
-        <v>80</v>
+      <c r="H14">
+        <v>0</v>
+      </c>
+      <c r="J14" t="s">
+        <v>76</v>
+      </c>
+      <c r="K14" t="s">
+        <v>79</v>
       </c>
       <c r="Q14" s="3"/>
     </row>
@@ -1262,27 +1207,27 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
+        <v>85</v>
+      </c>
+      <c r="C15" t="s">
         <v>8</v>
       </c>
-      <c r="C15">
-        <v>0</v>
-      </c>
-      <c r="D15" t="s">
-        <v>25</v>
+      <c r="D15">
+        <v>0</v>
       </c>
       <c r="E15" t="s">
         <v>25</v>
       </c>
-      <c r="F15">
-        <v>0</v>
+      <c r="F15" t="s">
+        <v>25</v>
       </c>
       <c r="G15">
         <v>0</v>
       </c>
-      <c r="I15" t="s">
-        <v>81</v>
-      </c>
-      <c r="K15" t="s">
+      <c r="H15">
+        <v>0</v>
+      </c>
+      <c r="J15" t="s">
         <v>76</v>
       </c>
       <c r="Q15" s="3"/>
@@ -1292,98 +1237,193 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
+        <v>74</v>
+      </c>
+      <c r="C16" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>25</v>
+      </c>
+      <c r="F16" t="s">
+        <v>83</v>
+      </c>
+      <c r="G16">
+        <v>0</v>
+      </c>
+      <c r="H16">
+        <v>0</v>
+      </c>
+      <c r="J16" t="s">
+        <v>76</v>
+      </c>
+      <c r="K16" t="s">
+        <v>79</v>
+      </c>
+      <c r="Q16" s="3"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>32</v>
+      </c>
+      <c r="C17" t="s">
+        <v>8</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>25</v>
+      </c>
+      <c r="F17" t="s">
+        <v>25</v>
+      </c>
+      <c r="G17">
+        <v>0</v>
+      </c>
+      <c r="H17">
+        <v>0</v>
+      </c>
+      <c r="J17" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q17" s="3"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>75</v>
+      </c>
+      <c r="C18" t="s">
+        <v>12</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18" t="s">
+        <v>25</v>
+      </c>
+      <c r="F18" t="s">
+        <v>25</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+      <c r="H18">
+        <v>0</v>
+      </c>
+      <c r="J18" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q18" s="3"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>71</v>
+      </c>
+      <c r="C19" t="s">
+        <v>8</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>25</v>
+      </c>
+      <c r="F19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19">
+        <v>0</v>
+      </c>
+      <c r="J19" t="s">
+        <v>76</v>
+      </c>
+      <c r="Q19" s="3"/>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>70</v>
+      </c>
+      <c r="C20" t="s">
         <v>14</v>
       </c>
-      <c r="C16">
-        <v>0</v>
-      </c>
-      <c r="D16" t="s">
-        <v>25</v>
-      </c>
-      <c r="E16" t="s">
-        <v>25</v>
-      </c>
-      <c r="F16">
-        <v>0</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="I16" t="s">
-        <v>81</v>
-      </c>
-      <c r="K16" t="s">
-        <v>75</v>
-      </c>
-      <c r="Q16" s="3"/>
-    </row>
-    <row r="17" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q17" s="3"/>
-    </row>
-    <row r="18" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q18" s="3"/>
-    </row>
-    <row r="19" spans="17:17" x14ac:dyDescent="0.25">
-      <c r="Q19" s="3"/>
-    </row>
-    <row r="21" spans="17:17" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20" t="s">
+        <v>25</v>
+      </c>
+      <c r="F20" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20">
+        <v>0</v>
+      </c>
+      <c r="H20">
+        <v>0</v>
+      </c>
+      <c r="J20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>86</v>
+      </c>
+      <c r="C21" t="s">
+        <v>87</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>25</v>
+      </c>
+      <c r="F21" t="s">
+        <v>25</v>
+      </c>
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0</v>
+      </c>
+      <c r="J21" t="s">
+        <v>76</v>
+      </c>
       <c r="Q21">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="Q1:XFD19 A107:XFD1048576 P20:XFD106 M1:O1 A1:K1">
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="2" priority="11">
       <formula>EXACT(TEXT(A1,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K4">
-    <cfRule type="expression" dxfId="9" priority="10">
-      <formula>EXACT(TEXT(K4,"text"),"?")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K5:K6">
-    <cfRule type="expression" dxfId="8" priority="9">
-      <formula>EXACT(TEXT(K5,"text"),"?")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6">
-    <cfRule type="expression" dxfId="7" priority="8">
-      <formula>EXACT(TEXT(B6,"text"),"?")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K7">
-    <cfRule type="expression" dxfId="6" priority="7">
-      <formula>EXACT(TEXT(K7,"text"),"?")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K9">
-    <cfRule type="expression" dxfId="5" priority="6">
-      <formula>EXACT(TEXT(K9,"text"),"?")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K11">
-    <cfRule type="expression" dxfId="4" priority="5">
-      <formula>EXACT(TEXT(K11,"text"),"?")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K12">
-    <cfRule type="expression" dxfId="3" priority="4">
-      <formula>EXACT(TEXT(K12,"text"),"?")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K13">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>EXACT(TEXT(K13,"text"),"?")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K14">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>EXACT(TEXT(K14,"text"),"?")</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A19:O106">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="A23:O24 A41:O106 A25:G40 I25:O40 L19:O22">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>EXACT(TEXT(A19,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1391,36 +1431,18 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$C$3:$C$13</xm:f>
+            <xm:f>Lists!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>E20:E36 B6</xm:sqref>
+          <xm:sqref>C6</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
-            <xm:f>Lists!$C$15:$C$19</xm:f>
+            <xm:f>Lists!#REF!</xm:f>
           </x14:formula1>
-          <xm:sqref>H20</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Lists!$C$20:$C$22</xm:f>
-          </x14:formula1>
-          <xm:sqref>H21</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Lists!$C$23:$C$28</xm:f>
-          </x14:formula1>
-          <xm:sqref>H27</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Lists!$C$29:$C$37</xm:f>
-          </x14:formula1>
-          <xm:sqref>H29</xm:sqref>
+          <xm:sqref>E23:E36</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1430,23 +1452,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.28515625" customWidth="1"/>
     <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.5703125" customWidth="1"/>
+    <col min="6" max="6" width="32" customWidth="1"/>
+    <col min="9" max="9" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>40</v>
       </c>
@@ -1466,7 +1489,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1486,27 +1509,27 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
-        <v>7</v>
+      <c r="C3" s="5" t="s">
+        <v>90</v>
       </c>
       <c r="D3">
         <v>0</v>
       </c>
-      <c r="E3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="E3" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1514,19 +1537,19 @@
         <v>9</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4" t="s">
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -1534,19 +1557,19 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="D5">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2</v>
       </c>
@@ -1554,19 +1577,19 @@
         <v>9</v>
       </c>
       <c r="C6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1574,19 +1597,19 @@
         <v>9</v>
       </c>
       <c r="C7" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="D7">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="F7" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2</v>
       </c>
@@ -1594,19 +1617,19 @@
         <v>9</v>
       </c>
       <c r="C8" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D8">
         <v>0</v>
       </c>
       <c r="E8" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="F8" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2</v>
       </c>
@@ -1614,19 +1637,19 @@
         <v>9</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1634,19 +1657,19 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>88</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2</v>
       </c>
@@ -1654,22 +1677,19 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="F11" t="s">
-        <v>13</v>
-      </c>
-      <c r="G11" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2</v>
       </c>
@@ -1677,19 +1697,19 @@
         <v>9</v>
       </c>
       <c r="C12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="D12">
         <v>0</v>
       </c>
       <c r="E12" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2</v>
       </c>
@@ -1709,7 +1729,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
@@ -1717,99 +1737,96 @@
         <v>9</v>
       </c>
       <c r="C14" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="D14">
         <v>0</v>
       </c>
       <c r="E14" t="s">
-        <v>70</v>
+        <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>70</v>
-      </c>
-      <c r="H14" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C15" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
       <c r="D15">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
+        <v>91</v>
       </c>
       <c r="F15" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C16" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="D16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>20</v>
+        <v>92</v>
       </c>
       <c r="F16" t="s">
-        <v>60</v>
+        <v>92</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="D17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E17" t="s">
-        <v>21</v>
+        <v>67</v>
       </c>
       <c r="F17" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B18" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="C18" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="D18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E18" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>61</v>
+        <v>13</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1820,156 +1837,156 @@
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F19" t="s">
-        <v>62</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B20" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C20" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D20">
         <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="F20" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D21">
         <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="F21" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C22" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="D22">
         <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="F22" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>49</v>
+        <v>18</v>
       </c>
       <c r="C23" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="D23">
         <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="F23" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="F24" t="s">
-        <v>53</v>
+        <v>62</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="F25" t="s">
-        <v>54</v>
+        <v>63</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B26" t="s">
-        <v>49</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="F26" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1977,19 +1994,19 @@
         <v>5</v>
       </c>
       <c r="B27" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C27" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="F27" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1997,99 +2014,99 @@
         <v>5</v>
       </c>
       <c r="B28" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C28" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="F28" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B29" t="s">
-        <v>51</v>
-      </c>
-      <c r="C29">
-        <v>1</v>
+        <v>47</v>
+      </c>
+      <c r="C29" t="s">
+        <v>52</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
-      <c r="E29">
-        <v>1</v>
-      </c>
-      <c r="F29">
-        <v>1</v>
+      <c r="E29" t="s">
+        <v>52</v>
+      </c>
+      <c r="F29" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B30" t="s">
-        <v>51</v>
-      </c>
-      <c r="C30">
-        <v>2</v>
+        <v>47</v>
+      </c>
+      <c r="C30" t="s">
+        <v>53</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
-      <c r="E30">
-        <v>2</v>
-      </c>
-      <c r="F30">
-        <v>2</v>
+      <c r="E30" t="s">
+        <v>53</v>
+      </c>
+      <c r="F30" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
-      </c>
-      <c r="C31">
-        <v>3</v>
+        <v>47</v>
+      </c>
+      <c r="C31" t="s">
+        <v>54</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
-      <c r="E31">
-        <v>3</v>
-      </c>
-      <c r="F31">
-        <v>3</v>
+      <c r="E31" t="s">
+        <v>54</v>
+      </c>
+      <c r="F31" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B32" t="s">
-        <v>51</v>
-      </c>
-      <c r="C32">
-        <v>4</v>
+        <v>47</v>
+      </c>
+      <c r="C32" t="s">
+        <v>55</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
-      <c r="E32">
-        <v>4</v>
-      </c>
-      <c r="F32">
-        <v>4</v>
+      <c r="E32" t="s">
+        <v>55</v>
+      </c>
+      <c r="F32" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -2097,19 +2114,19 @@
         <v>6</v>
       </c>
       <c r="B33" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C33">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D33">
         <v>1</v>
       </c>
       <c r="E33">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F33">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -2117,19 +2134,19 @@
         <v>6</v>
       </c>
       <c r="B34" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C34">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D34">
         <v>1</v>
       </c>
       <c r="E34">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="F34">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -2137,19 +2154,19 @@
         <v>6</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C35">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="D35">
         <v>1</v>
       </c>
       <c r="E35">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="F35">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -2157,19 +2174,19 @@
         <v>6</v>
       </c>
       <c r="B36" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C36">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D36">
         <v>1</v>
       </c>
       <c r="E36">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="F36">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -2177,18 +2194,98 @@
         <v>6</v>
       </c>
       <c r="B37" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C37">
+        <v>5</v>
+      </c>
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>5</v>
+      </c>
+      <c r="F37">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>6</v>
+      </c>
+      <c r="B38" t="s">
+        <v>49</v>
+      </c>
+      <c r="C38">
+        <v>6</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>6</v>
+      </c>
+      <c r="F38">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>6</v>
+      </c>
+      <c r="B39" t="s">
+        <v>49</v>
+      </c>
+      <c r="C39">
+        <v>7</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>7</v>
+      </c>
+      <c r="F39">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40">
+        <v>6</v>
+      </c>
+      <c r="B40" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40">
+        <v>8</v>
+      </c>
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>8</v>
+      </c>
+      <c r="F40">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41">
+        <v>6</v>
+      </c>
+      <c r="B41" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41">
         <v>9</v>
       </c>
-      <c r="D37">
-        <v>1</v>
-      </c>
-      <c r="E37">
+      <c r="D41">
+        <v>1</v>
+      </c>
+      <c r="E41">
         <v>9</v>
       </c>
-      <c r="F37">
+      <c r="F41">
         <v>9</v>
       </c>
     </row>
@@ -2230,7 +2327,7 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
add validation attributes for default value
</commit_message>
<xml_diff>
--- a/Authentication.WEB/ExcelConfig/config_file.xlsx
+++ b/Authentication.WEB/ExcelConfig/config_file.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9090" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Item_Details" sheetId="1" r:id="rId1"/>
     <sheet name="Lists" sheetId="2" r:id="rId2"/>
     <sheet name="Name_caption_translation" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
+    <sheet name="Example" sheetId="5" r:id="rId4"/>
+    <sheet name="Dget" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="106">
   <si>
     <t>Field_ID</t>
   </si>
@@ -306,13 +307,52 @@
   </si>
   <si>
     <t>password</t>
+  </si>
+  <si>
+    <t>Courses</t>
+  </si>
+  <si>
+    <t>Trainings</t>
+  </si>
+  <si>
+    <t>Prices</t>
+  </si>
+  <si>
+    <t>Tax</t>
+  </si>
+  <si>
+    <t>CourseFee</t>
+  </si>
+  <si>
+    <t>Excel</t>
+  </si>
+  <si>
+    <t>Power Point</t>
+  </si>
+  <si>
+    <t>Word</t>
+  </si>
+  <si>
+    <t>Access</t>
+  </si>
+  <si>
+    <t>Project</t>
+  </si>
+  <si>
+    <t>Course Fee</t>
+  </si>
+  <si>
+    <t>Basic</t>
+  </si>
+  <si>
+    <t>Advanced</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -330,8 +370,15 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -341,6 +388,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -385,7 +438,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -394,21 +447,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color auto="1"/>
@@ -741,7 +785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="O20" sqref="O20"/>
     </sheetView>
   </sheetViews>
@@ -1418,12 +1462,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="Q1:XFD19 A107:XFD1048576 P20:XFD106 M1:O1 A1:K1">
-    <cfRule type="expression" dxfId="2" priority="11">
+    <cfRule type="expression" dxfId="1" priority="11">
       <formula>EXACT(TEXT(A1,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A23:O24 A41:O106 A25:G40 I25:O40 L19:O22">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>EXACT(TEXT(A19,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1454,7 +1498,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
@@ -2370,14 +2414,240 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2">
+        <v>4500</v>
+      </c>
+      <c r="D2">
+        <v>0.12</v>
+      </c>
+      <c r="E2">
+        <v>5040</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C3">
+        <v>5500</v>
+      </c>
+      <c r="D3">
+        <v>0.12</v>
+      </c>
+      <c r="E3">
+        <v>6160</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4">
+        <v>3000</v>
+      </c>
+      <c r="D4">
+        <v>0.12</v>
+      </c>
+      <c r="E4">
+        <v>3360</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C5">
+        <v>4500</v>
+      </c>
+      <c r="D5">
+        <v>0.12</v>
+      </c>
+      <c r="E5">
+        <v>5040</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6" t="s">
+        <v>104</v>
+      </c>
+      <c r="C6">
+        <v>3000</v>
+      </c>
+      <c r="D6">
+        <v>0.12</v>
+      </c>
+      <c r="E6">
+        <v>3360</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>100</v>
+      </c>
+      <c r="B7" t="s">
+        <v>105</v>
+      </c>
+      <c r="C7">
+        <v>4500</v>
+      </c>
+      <c r="D7">
+        <v>0.12</v>
+      </c>
+      <c r="E7">
+        <v>5040</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" t="s">
+        <v>104</v>
+      </c>
+      <c r="C8">
+        <v>4500</v>
+      </c>
+      <c r="D8">
+        <v>0.12</v>
+      </c>
+      <c r="E8">
+        <v>5040</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B9" t="s">
+        <v>105</v>
+      </c>
+      <c r="C9">
+        <v>7000</v>
+      </c>
+      <c r="D9">
+        <v>0.12</v>
+      </c>
+      <c r="E9">
+        <v>7840</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B10" t="s">
+        <v>104</v>
+      </c>
+      <c r="C10">
+        <v>4500</v>
+      </c>
+      <c r="D10">
+        <v>0.12</v>
+      </c>
+      <c r="E10">
+        <v>5040</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C11">
+        <v>7000</v>
+      </c>
+      <c r="D11">
+        <v>0.12</v>
+      </c>
+      <c r="E11">
+        <v>7840</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>98</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2">
+        <f>DGET(Example!A1:E11, Example!E1,A1:B2)</f>
+        <v>6160</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
if function parsing prototype
</commit_message>
<xml_diff>
--- a/Authentication.WEB/ExcelConfig/config_file.xlsx
+++ b/Authentication.WEB/ExcelConfig/config_file.xlsx
@@ -3799,11 +3799,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q34"/>
+  <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O12" sqref="O12"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O19" sqref="O19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4808,7 +4808,7 @@
         <v>2</v>
       </c>
       <c r="P23" s="3">
-        <f ca="1">P22-O29</f>
+        <f ca="1">P22-O30</f>
         <v>3345.4375</v>
       </c>
       <c r="Q23" s="114"/>
@@ -4850,66 +4850,39 @@
         <v>2</v>
       </c>
       <c r="P24" s="3">
-        <f ca="1">P23-P23*M28</f>
+        <f ca="1">P23-P23*M29</f>
         <v>2509.078125</v>
       </c>
       <c r="Q24" s="114"/>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A25" s="103">
-        <v>24</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>68</v>
-      </c>
+      <c r="A25" s="103"/>
+      <c r="B25" s="3"/>
       <c r="C25" s="3"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" s="8">
-        <v>8</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="I25" s="3">
-        <v>0</v>
-      </c>
-      <c r="J25" s="3">
-        <v>1</v>
-      </c>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
       <c r="K25" s="3"/>
-      <c r="L25" s="10" t="s">
-        <v>159</v>
-      </c>
-      <c r="M25" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="N25" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="O25" s="3">
-        <f>DGET(DGET!A386:C426,"NCD",DGET!A429:C430)</f>
-        <v>0.3</v>
-      </c>
+      <c r="L25" s="10"/>
+      <c r="M25" s="4"/>
+      <c r="N25" s="3"/>
+      <c r="O25" s="3"/>
       <c r="P25" s="3">
-        <f ca="1">P24-P24*O25</f>
-        <v>1756.3546875000002</v>
-      </c>
-      <c r="Q25" s="114" t="s">
-        <v>161</v>
-      </c>
+        <f ca="1">P24*O26</f>
+        <v>752.72343749999993</v>
+      </c>
+      <c r="Q25" s="114"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A26" s="103">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>140</v>
+        <v>68</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="5"/>
@@ -4917,13 +4890,13 @@
         <v>26</v>
       </c>
       <c r="F26" s="8">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>151</v>
+        <v>79</v>
       </c>
       <c r="H26" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="I26" s="3">
         <v>0</v>
@@ -4933,54 +4906,64 @@
       </c>
       <c r="K26" s="3"/>
       <c r="L26" s="10" t="s">
-        <v>140</v>
+        <v>159</v>
       </c>
       <c r="M26" s="3" t="s">
-        <v>82</v>
+        <v>154</v>
       </c>
       <c r="N26" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="O26" s="23" t="s">
-        <v>2</v>
-      </c>
-      <c r="P26" s="3"/>
-      <c r="Q26" s="114"/>
+        <v>179</v>
+      </c>
+      <c r="O26" s="3">
+        <f>DGET(DGET!A386:C426,"NCD",DGET!A429:C430)</f>
+        <v>0.3</v>
+      </c>
+      <c r="P26" s="3">
+        <f ca="1">P24-P25</f>
+        <v>1756.3546875000002</v>
+      </c>
+      <c r="Q26" s="114" t="s">
+        <v>161</v>
+      </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="103">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>69</v>
+        <v>140</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="5"/>
-      <c r="E27" s="8" t="s">
-        <v>7</v>
+      <c r="E27" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="F27" s="8">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="H27" s="8" t="s">
-        <v>74</v>
+        <v>151</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>82</v>
       </c>
       <c r="I27" s="3">
         <v>0</v>
       </c>
       <c r="J27" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K27" s="3"/>
-      <c r="L27" s="10"/>
-      <c r="M27" s="3"/>
+      <c r="L27" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="M27" s="3" t="s">
+        <v>82</v>
+      </c>
       <c r="N27" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="O27" s="3" t="s">
+      <c r="O27" s="23" t="s">
         <v>2</v>
       </c>
       <c r="P27" s="3"/>
@@ -4988,40 +4971,36 @@
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A28" s="103">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="5"/>
-      <c r="E28" s="3" t="s">
-        <v>26</v>
+      <c r="E28" s="8" t="s">
+        <v>7</v>
       </c>
       <c r="F28" s="8">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="H28" s="4">
-        <v>0</v>
+        <v>72</v>
+      </c>
+      <c r="H28" s="8" t="s">
+        <v>74</v>
       </c>
       <c r="I28" s="3">
         <v>0</v>
       </c>
       <c r="J28" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K28" s="3"/>
-      <c r="L28" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="M28" s="4">
-        <v>0.25</v>
-      </c>
+      <c r="L28" s="10"/>
+      <c r="M28" s="3"/>
       <c r="N28" s="3" t="s">
-        <v>181</v>
+        <v>2</v>
       </c>
       <c r="O28" s="3" t="s">
         <v>2</v>
@@ -5031,130 +5010,172 @@
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A29" s="103">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="5"/>
       <c r="E29" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="F29" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" s="8">
+        <v>10</v>
+      </c>
+      <c r="G29" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="H29" s="4">
+        <v>0</v>
+      </c>
+      <c r="I29" s="3">
+        <v>0</v>
+      </c>
+      <c r="J29" s="3">
+        <v>1</v>
+      </c>
+      <c r="K29" s="3"/>
+      <c r="L29" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="M29" s="4">
+        <v>0.25</v>
+      </c>
+      <c r="N29" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="O29" s="3" t="s">
         <v>2</v>
-      </c>
-      <c r="G29" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H29" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I29" s="3">
-        <v>0</v>
-      </c>
-      <c r="J29" s="3">
-        <v>1</v>
-      </c>
-      <c r="K29" s="3"/>
-      <c r="L29" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="M29" s="4">
-        <v>25</v>
-      </c>
-      <c r="N29" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="O29" s="3">
-        <v>3</v>
       </c>
       <c r="P29" s="3"/>
       <c r="Q29" s="114"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A30" s="104">
-        <v>29</v>
+      <c r="A30" s="103">
+        <v>28</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="5"/>
-      <c r="E30" s="8" t="s">
+      <c r="E30" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="F30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I30" s="3">
+        <v>0</v>
+      </c>
+      <c r="J30" s="3">
+        <v>1</v>
+      </c>
+      <c r="K30" s="3"/>
+      <c r="L30" s="8" t="s">
+        <v>165</v>
+      </c>
+      <c r="M30" s="4">
+        <v>25</v>
+      </c>
+      <c r="N30" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="O30" s="3">
+        <v>3</v>
+      </c>
+      <c r="P30" s="3">
+        <f ca="1">P26*1.01</f>
+        <v>1773.9182343750001</v>
+      </c>
+      <c r="Q30" s="114"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A31" s="104">
+        <v>29</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="F30" s="8">
+      <c r="F31" s="8">
         <v>7</v>
       </c>
-      <c r="G30" s="3" t="s">
+      <c r="G31" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="H30" s="8" t="s">
+      <c r="H31" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="I30" s="5">
-        <v>0</v>
-      </c>
-      <c r="J30" s="5">
-        <v>1</v>
-      </c>
-      <c r="K30" s="3"/>
-      <c r="L30" s="32" t="s">
+      <c r="I31" s="5">
+        <v>0</v>
+      </c>
+      <c r="J31" s="5">
+        <v>1</v>
+      </c>
+      <c r="K31" s="3"/>
+      <c r="L31" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="M30" s="8" t="s">
+      <c r="M31" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="N30" s="5" t="s">
+      <c r="N31" s="5" t="s">
         <v>183</v>
       </c>
-      <c r="O30" s="3">
-        <f ca="1">P25+P25*0.01</f>
+      <c r="P31" s="3">
+        <f ca="1">IF(M31="yes",P30,P26)</f>
         <v>1773.9182343750001</v>
       </c>
-      <c r="P30" s="3">
-        <f ca="1">IF(M30="yes",O30,P25)</f>
-        <v>1773.9182343750001</v>
-      </c>
-      <c r="Q30" s="114"/>
-    </row>
-    <row r="31" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="115"/>
-      <c r="B31" s="43"/>
-      <c r="C31" s="43"/>
-      <c r="D31" s="43"/>
-      <c r="E31" s="43"/>
-      <c r="F31" s="43"/>
-      <c r="G31" s="43"/>
-      <c r="H31" s="43"/>
-      <c r="I31" s="43"/>
-      <c r="J31" s="43"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="43"/>
-      <c r="M31" s="43"/>
-      <c r="N31" s="58" t="s">
+      <c r="Q31" s="114"/>
+    </row>
+    <row r="32" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="115"/>
+      <c r="B32" s="43"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="43"/>
+      <c r="I32" s="43"/>
+      <c r="J32" s="43"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="43"/>
+      <c r="M32" s="43"/>
+      <c r="N32" s="58" t="s">
         <v>214</v>
       </c>
-      <c r="O31" s="43">
-        <v>0</v>
-      </c>
-      <c r="P31" s="43">
-        <f ca="1">ROUND(P30,O31)</f>
+      <c r="O32" s="43">
+        <v>0</v>
+      </c>
+      <c r="P32" s="43">
+        <f ca="1">ROUND(P31,O32)</f>
         <v>1774</v>
       </c>
-      <c r="Q31" s="14"/>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="N32" s="149"/>
-    </row>
-    <row r="34" spans="11:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="K34" s="148" t="s">
+      <c r="Q32" s="14"/>
+    </row>
+    <row r="33" spans="11:14" x14ac:dyDescent="0.25">
+      <c r="N33" s="149"/>
+    </row>
+    <row r="35" spans="11:14" ht="45" x14ac:dyDescent="0.25">
+      <c r="K35" s="148" t="s">
         <v>239</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="P13:XFD13 O12:XFD12 M31:XFD1048576 O14:XFD14 P8:XFD9 Q10:XFD10 P2:P7 V2:XFD7 M1:Q1 S15:XFD15 O15:Q15 S11:XFD11 P11:Q11 AC1:XFD1 P26:XFD26 Q30:XFD30 M30:O30 O16:XFD25 M12:M17 M19:M30 K1 L19:L1048576 L1:L17 A1:J1048576 N27:XFD29 N12:N25 O2:O11">
+  <conditionalFormatting sqref="P13:XFD13 O12:XFD12 M32:XFD1048576 O14:XFD14 P8:XFD9 Q10:XFD10 P2:P7 V2:XFD7 M1:Q1 S15:XFD15 O15:Q15 S11:XFD11 P11:Q11 AC1:XFD1 P27:XFD27 O16:XFD26 M12:M17 M19:M31 K1 L19:L1048576 L1:L17 A1:J1048576 N28:XFD29 N12:N26 O2:O11 Q30:XFD31 M31:N31 N30:P30">
     <cfRule type="expression" dxfId="15" priority="8">
       <formula>EXACT(TEXT(A1,"text"),"?")</formula>
     </cfRule>
@@ -5184,13 +5205,13 @@
       <formula>EXACT(TEXT(L18,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="N26">
+  <conditionalFormatting sqref="N27">
     <cfRule type="expression" dxfId="9" priority="1">
-      <formula>EXACT(TEXT(N26,"text"),"?")</formula>
+      <formula>EXACT(TEXT(N27,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H27 H30 H22 M26 M28">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H28 H31 H22 M27 M29">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -5198,7 +5219,7 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="8">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="8">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lists!$C$14:$C$18</xm:f>
@@ -5221,31 +5242,31 @@
           <x14:formula1>
             <xm:f>Lists!$C$29:$C$30</xm:f>
           </x14:formula1>
-          <xm:sqref>H19:H20 M19:M20 M22:M23 M30</xm:sqref>
+          <xm:sqref>H19:H20 M19:M20 M22:M23 M31</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lists!$C$3:$C$18</xm:f>
           </x14:formula1>
-          <xm:sqref>E2:E22 E24:E30</xm:sqref>
+          <xm:sqref>E2:E22 E24:E31</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lists!$C$49:$C$56</xm:f>
           </x14:formula1>
-          <xm:sqref>H26</xm:sqref>
+          <xm:sqref>H27</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lists!$C$32:$C$38</xm:f>
           </x14:formula1>
-          <xm:sqref>H25 M25</xm:sqref>
+          <xm:sqref>H26 M26</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Lists!$C$31:$C$44</xm:f>
           </x14:formula1>
-          <xm:sqref>H28</xm:sqref>
+          <xm:sqref>H29</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -10809,7 +10830,7 @@
         <v>Motorcycle</v>
       </c>
       <c r="B430" s="50" t="str">
-        <f>ConfigurationSetup!M25</f>
+        <f>ConfigurationSetup!M26</f>
         <v>1 Year - 30</v>
       </c>
       <c r="C430" s="39"/>

</xml_diff>

<commit_message>
exact and round functions parsed
</commit_message>
<xml_diff>
--- a/Authentication.WEB/ExcelConfig/config_file.xlsx
+++ b/Authentication.WEB/ExcelConfig/config_file.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1704" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1711" uniqueCount="252">
   <si>
     <t>Default</t>
   </si>
@@ -783,6 +783,12 @@
   </si>
   <si>
     <t>RatingIndicator</t>
+  </si>
+  <si>
+    <t>туј пада зш е нулл</t>
+  </si>
+  <si>
+    <t>Calc_rates</t>
   </si>
 </sst>
 </file>
@@ -1616,7 +1622,37 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="19">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -3802,8 +3838,8 @@
   <dimension ref="A1:Q35"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O19" sqref="O19"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P29" sqref="P29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3916,8 +3952,8 @@
       <c r="O2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="P2" s="3">
-        <v>0</v>
+      <c r="P2" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="Q2" s="114"/>
     </row>
@@ -3959,7 +3995,8 @@
         <v>2</v>
       </c>
       <c r="P3" s="3">
-        <v>0</v>
+        <f>O13*100</f>
+        <v>400</v>
       </c>
       <c r="Q3" s="114"/>
     </row>
@@ -4000,7 +4037,10 @@
       <c r="O4" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="P4" s="3"/>
+      <c r="P4" s="3">
+        <f>O11+P3</f>
+        <v>1650</v>
+      </c>
       <c r="Q4" s="114"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
@@ -4040,7 +4080,10 @@
       <c r="O5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="P5" s="3"/>
+      <c r="P5" s="3">
+        <f ca="1">P4*O14</f>
+        <v>0</v>
+      </c>
       <c r="Q5" s="114"/>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
@@ -4076,7 +4119,10 @@
       <c r="O6" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="P6" s="3"/>
+      <c r="P6" s="3">
+        <f ca="1">P4+P5</f>
+        <v>1650</v>
+      </c>
       <c r="Q6" s="114"/>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
@@ -4116,7 +4162,10 @@
       <c r="O7" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="P7" s="3"/>
+      <c r="P7" s="3">
+        <f ca="1">IF(P6&gt;O15,P6,O15)</f>
+        <v>1650</v>
+      </c>
       <c r="Q7" s="114"/>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
@@ -4152,7 +4201,10 @@
       <c r="O8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="P8" s="3"/>
+      <c r="P8" s="3">
+        <f ca="1">O16*P7</f>
+        <v>165</v>
+      </c>
       <c r="Q8" s="114"/>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
@@ -4188,7 +4240,10 @@
       <c r="O9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="P9" s="3"/>
+      <c r="P9" s="3">
+        <f ca="1">P8+P7</f>
+        <v>1815</v>
+      </c>
       <c r="Q9" s="114"/>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -4224,7 +4279,10 @@
       <c r="O10" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="P10" s="3"/>
+      <c r="P10" s="3">
+        <f ca="1">P9+O17</f>
+        <v>2015</v>
+      </c>
       <c r="Q10" s="114"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -4261,12 +4319,16 @@
       <c r="M11" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="O11" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="P11" s="3">
+      <c r="N11" t="s">
+        <v>251</v>
+      </c>
+      <c r="O11" s="3">
         <f>DGET(DGET!A1:C36,"Rates",DGET!A39:C40)</f>
         <v>1250</v>
+      </c>
+      <c r="P11">
+        <f ca="1">P10*O18</f>
+        <v>0</v>
       </c>
       <c r="Q11" s="114" t="s">
         <v>110</v>
@@ -4313,7 +4375,10 @@
         <f>M12-5</f>
         <v>2</v>
       </c>
-      <c r="P12" s="3"/>
+      <c r="P12" s="3">
+        <f ca="1">P10-P11</f>
+        <v>2015</v>
+      </c>
       <c r="Q12" s="114"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
@@ -4357,9 +4422,9 @@
         <f>M13-1</f>
         <v>4</v>
       </c>
-      <c r="P13" s="3">
-        <f>P11+O13*100</f>
-        <v>1650</v>
+      <c r="P13">
+        <f ca="1">P12*O19</f>
+        <v>503.75</v>
       </c>
       <c r="Q13" s="114"/>
     </row>
@@ -4401,8 +4466,8 @@
         <v>0</v>
       </c>
       <c r="P14" s="3">
-        <f ca="1">P13+P13*O14</f>
-        <v>1650</v>
+        <f ca="1">P12+P13</f>
+        <v>2518.75</v>
       </c>
       <c r="Q14" s="114" t="s">
         <v>135</v>
@@ -4445,9 +4510,9 @@
         <f>DGET(DGET!A138:D243,"min_premium",DGET!A246:D247)</f>
         <v>0</v>
       </c>
-      <c r="P15" s="3">
-        <f ca="1">IF(P14&gt;O15,P14,O15)</f>
-        <v>1650</v>
+      <c r="P15">
+        <f ca="1">P14*O20</f>
+        <v>629.6875</v>
       </c>
       <c r="Q15" s="114" t="s">
         <v>137</v>
@@ -4491,8 +4556,8 @@
         <v>0.1</v>
       </c>
       <c r="P16" s="3">
-        <f ca="1">O16*P15+P15</f>
-        <v>1815</v>
+        <f ca="1">P14+P15</f>
+        <v>3148.4375</v>
       </c>
       <c r="Q16" s="114" t="s">
         <v>138</v>
@@ -4536,8 +4601,8 @@
         <v>200</v>
       </c>
       <c r="P17" s="3">
-        <f ca="1">P16+O17</f>
-        <v>2015</v>
+        <f ca="1">P16+O21</f>
+        <v>3348.4375</v>
       </c>
       <c r="Q17" s="114"/>
     </row>
@@ -4578,9 +4643,8 @@
         <f>DGET(DGET!A260:D380,"CMP",DGET!A383:D384)</f>
         <v>0</v>
       </c>
-      <c r="P18" s="3">
-        <f ca="1">P17-P17*O18</f>
-        <v>2015</v>
+      <c r="P18" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="Q18" s="114" t="s">
         <v>152</v>
@@ -4627,9 +4691,9 @@
         <f>IF(M19="yes",0.25,0)</f>
         <v>0.25</v>
       </c>
-      <c r="P19" s="3">
-        <f ca="1">P18+P18*O19</f>
-        <v>2518.75</v>
+      <c r="P19">
+        <f>O22+1</f>
+        <v>1</v>
       </c>
       <c r="Q19" s="114"/>
     </row>
@@ -4675,8 +4739,8 @@
         <v>0.25</v>
       </c>
       <c r="P20" s="3">
-        <f ca="1">P19+P19*O20</f>
-        <v>3148.4375</v>
+        <f ca="1">P17*P19</f>
+        <v>3348.4375</v>
       </c>
       <c r="Q20" s="114"/>
     </row>
@@ -4719,8 +4783,8 @@
         <v>200</v>
       </c>
       <c r="P21" s="3">
-        <f ca="1">P20+O21</f>
-        <v>3348.4375</v>
+        <f ca="1">P20-O30</f>
+        <v>3345.4375</v>
       </c>
       <c r="Q21" s="114"/>
     </row>
@@ -4765,9 +4829,9 @@
         <f>IF(M22="yes",1,0)</f>
         <v>0</v>
       </c>
-      <c r="P22" s="3">
-        <f ca="1">P21*O22+P21</f>
-        <v>3348.4375</v>
+      <c r="P22">
+        <f ca="1">P21*O25</f>
+        <v>836.359375</v>
       </c>
       <c r="Q22" s="114"/>
     </row>
@@ -4808,8 +4872,8 @@
         <v>2</v>
       </c>
       <c r="P23" s="3">
-        <f ca="1">P22-O30</f>
-        <v>3345.4375</v>
+        <f ca="1">P21-P22</f>
+        <v>2509.078125</v>
       </c>
       <c r="Q23" s="114"/>
     </row>
@@ -4850,8 +4914,8 @@
         <v>2</v>
       </c>
       <c r="P24" s="3">
-        <f ca="1">P23-P23*M29</f>
-        <v>2509.078125</v>
+        <f ca="1">P23*O26</f>
+        <v>752.72343749999993</v>
       </c>
       <c r="Q24" s="114"/>
     </row>
@@ -4869,11 +4933,15 @@
       <c r="K25" s="3"/>
       <c r="L25" s="10"/>
       <c r="M25" s="4"/>
-      <c r="N25" s="3"/>
-      <c r="O25" s="3"/>
-      <c r="P25" s="3">
-        <f ca="1">P24*O26</f>
-        <v>752.72343749999993</v>
+      <c r="N25" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="O25" s="3">
+        <f>M29*1</f>
+        <v>0.25</v>
+      </c>
+      <c r="P25" s="3" t="s">
+        <v>2</v>
       </c>
       <c r="Q25" s="114"/>
     </row>
@@ -4919,7 +4987,7 @@
         <v>0.3</v>
       </c>
       <c r="P26" s="3">
-        <f ca="1">P24-P25</f>
+        <f ca="1">P23-P24</f>
         <v>1756.3546875000002</v>
       </c>
       <c r="Q26" s="114" t="s">
@@ -4966,7 +5034,9 @@
       <c r="O27" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="P27" s="3"/>
+      <c r="P27" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="Q27" s="114"/>
     </row>
     <row r="28" spans="1:17" x14ac:dyDescent="0.25">
@@ -5005,7 +5075,9 @@
       <c r="O28" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="P28" s="3"/>
+      <c r="P28" s="3" t="s">
+        <v>2</v>
+      </c>
       <c r="Q28" s="114"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
@@ -5048,7 +5120,10 @@
       <c r="O29" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="P29" s="3"/>
+      <c r="P29" s="3" t="b">
+        <f>EXACT(O29,O28)</f>
+        <v>1</v>
+      </c>
       <c r="Q29" s="114"/>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
@@ -5175,39 +5250,54 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="P13:XFD13 O12:XFD12 M32:XFD1048576 O14:XFD14 P8:XFD9 Q10:XFD10 P2:P7 V2:XFD7 M1:Q1 S15:XFD15 O15:Q15 S11:XFD11 P11:Q11 AC1:XFD1 P27:XFD27 O16:XFD26 M12:M17 M19:M31 K1 L19:L1048576 L1:L17 A1:J1048576 N28:XFD29 N12:N26 O2:O11 Q30:XFD31 M31:N31 N30:P30">
-    <cfRule type="expression" dxfId="15" priority="8">
+  <conditionalFormatting sqref="M32:XFD1048576 V2:XFD7 M1:Q1 S15:XFD15 S11:XFD11 AC1:XFD1 M12:M17 M19:M31 K1 L19:L1048576 L1:L17 A1:J1048576 N12:N24 Q30:XFD31 M31:N31 N30:P30 Q11 Q15 P8:XFD10 Q12:XFD14 P12 P14 Q16:XFD25 O14:O24 P23:P24 P16:P17 P20:P21 O2:O12 P2:P7 P27:XFD27 N28:XFD29 N26:XFD26">
+    <cfRule type="expression" dxfId="18" priority="11">
       <formula>EXACT(TEXT(A1,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M3:M10">
-    <cfRule type="expression" dxfId="14" priority="7">
+    <cfRule type="expression" dxfId="17" priority="10">
       <formula>EXACT(TEXT(M3,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11">
-    <cfRule type="expression" dxfId="13" priority="6">
+    <cfRule type="expression" dxfId="16" priority="9">
       <formula>EXACT(TEXT(M11,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2">
-    <cfRule type="expression" dxfId="12" priority="4">
+    <cfRule type="expression" dxfId="15" priority="7">
       <formula>EXACT(TEXT(M2,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M18">
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="14" priority="6">
       <formula>EXACT(TEXT(M18,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18">
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="13" priority="5">
       <formula>EXACT(TEXT(L18,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N27">
+    <cfRule type="expression" dxfId="12" priority="4">
+      <formula>EXACT(TEXT(N27,"text"),"?")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P18">
+    <cfRule type="expression" dxfId="11" priority="3">
+      <formula>EXACT(TEXT(P18,"text"),"?")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P25">
+    <cfRule type="expression" dxfId="10" priority="2">
+      <formula>EXACT(TEXT(P25,"text"),"?")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="N25:O25">
     <cfRule type="expression" dxfId="9" priority="1">
-      <formula>EXACT(TEXT(N27,"text"),"?")</formula>
+      <formula>EXACT(TEXT(N25,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
@@ -5276,10 +5366,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D430"/>
+  <dimension ref="A1:E430"/>
   <sheetViews>
-    <sheetView topLeftCell="A421" workbookViewId="0">
-      <selection activeCell="A433" sqref="A433"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="D136" sqref="D136"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6935,7 +7025,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="36" t="s">
         <v>106</v>
       </c>
@@ -6949,7 +7039,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="36" t="s">
         <v>106</v>
       </c>
@@ -6963,7 +7053,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="36" t="s">
         <v>106</v>
       </c>
@@ -6977,7 +7067,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="132" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="87" t="s">
         <v>106</v>
       </c>
@@ -6991,8 +7081,8 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="133" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="161" t="s">
         <v>86</v>
       </c>
@@ -7000,7 +7090,7 @@
       <c r="C134" s="162"/>
       <c r="D134" s="163"/>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="47" t="s">
         <v>15</v>
       </c>
@@ -7014,7 +7104,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="136" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="75" t="str">
         <f>ConfigurationSetup!M3</f>
         <v>Motorcycle</v>
@@ -7028,9 +7118,12 @@
         <v>Vehicle &lt;= 3 years</v>
       </c>
       <c r="D136" s="77"/>
-    </row>
-    <row r="137" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E136" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="137" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="26" t="s">
         <v>15</v>
       </c>
@@ -7044,7 +7137,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" s="28" t="s">
         <v>83</v>
       </c>
@@ -7058,7 +7151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" s="56" t="s">
         <v>83</v>
       </c>
@@ -7072,7 +7165,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" s="28" t="s">
         <v>83</v>
       </c>
@@ -7086,7 +7179,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" s="28" t="s">
         <v>83</v>
       </c>
@@ -7100,7 +7193,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" s="28" t="s">
         <v>83</v>
       </c>
@@ -7114,7 +7207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" s="28" t="s">
         <v>83</v>
       </c>
@@ -10890,7 +10983,7 @@
       </c>
       <c r="B3" s="41">
         <f ca="1">TODAY()</f>
-        <v>42821</v>
+        <v>42828</v>
       </c>
       <c r="C3" s="3">
         <f>IF(B$9&lt;B2,1,0)</f>
@@ -10903,7 +10996,7 @@
       </c>
       <c r="B4" s="41">
         <f ca="1">B3-1</f>
-        <v>42820</v>
+        <v>42827</v>
       </c>
       <c r="C4" s="3">
         <f ca="1">IF(B$9&lt;B3,1,0)</f>
@@ -10916,7 +11009,7 @@
       </c>
       <c r="B5" s="41">
         <f ca="1">EDATE(B3,-12)</f>
-        <v>42456</v>
+        <v>42463</v>
       </c>
       <c r="C5" s="3">
         <f ca="1">IF(B$9&lt;B5,1,0)</f>
@@ -10929,7 +11022,7 @@
       </c>
       <c r="B6" s="41">
         <f ca="1">EDATE(B3,-24)</f>
-        <v>42090</v>
+        <v>42097</v>
       </c>
       <c r="C6" s="3">
         <f ca="1">IF(B$9&lt;B6,1,0)</f>
@@ -10942,7 +11035,7 @@
       </c>
       <c r="B7" s="41">
         <f ca="1">EDATE(B3,-36)</f>
-        <v>41725</v>
+        <v>41732</v>
       </c>
       <c r="C7" s="3">
         <f ca="1">IF(B$9&lt;B7,1,0)</f>

</xml_diff>

<commit_message>
saving column for textbox in db
</commit_message>
<xml_diff>
--- a/Authentication.WEB/ExcelConfig/config_file.xlsx
+++ b/Authentication.WEB/ExcelConfig/config_file.xlsx
@@ -20,7 +20,6 @@
     <sheet name="FES2_CC" sheetId="15" r:id="rId6"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -3838,9 +3837,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P16" sqref="P16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10984,7 +10983,7 @@
       </c>
       <c r="B3" s="41">
         <f ca="1">TODAY()</f>
-        <v>42831</v>
+        <v>42847</v>
       </c>
       <c r="C3" s="3">
         <f>IF(B$9&lt;B2,1,0)</f>
@@ -10997,7 +10996,7 @@
       </c>
       <c r="B4" s="41">
         <f ca="1">B3-1</f>
-        <v>42830</v>
+        <v>42846</v>
       </c>
       <c r="C4" s="3">
         <f ca="1">IF(B$9&lt;B3,1,0)</f>
@@ -11010,7 +11009,7 @@
       </c>
       <c r="B5" s="41">
         <f ca="1">EDATE(B3,-12)</f>
-        <v>42466</v>
+        <v>42482</v>
       </c>
       <c r="C5" s="3">
         <f ca="1">IF(B$9&lt;B5,1,0)</f>
@@ -11023,7 +11022,7 @@
       </c>
       <c r="B6" s="41">
         <f ca="1">EDATE(B3,-24)</f>
-        <v>42100</v>
+        <v>42116</v>
       </c>
       <c r="C6" s="3">
         <f ca="1">IF(B$9&lt;B6,1,0)</f>
@@ -11036,7 +11035,7 @@
       </c>
       <c r="B7" s="41">
         <f ca="1">EDATE(B3,-36)</f>
-        <v>41735</v>
+        <v>41751</v>
       </c>
       <c r="C7" s="3">
         <f ca="1">IF(B$9&lt;B7,1,0)</f>

</xml_diff>

<commit_message>
bug fix - changes in if procedures in master procedure
</commit_message>
<xml_diff>
--- a/Authentication.WEB/ExcelConfig/config_file.xlsx
+++ b/Authentication.WEB/ExcelConfig/config_file.xlsx
@@ -699,9 +699,6 @@
     <t>Special percent</t>
   </si>
   <si>
-    <t xml:space="preserve">NCD </t>
-  </si>
-  <si>
     <t>ne</t>
   </si>
   <si>
@@ -802,6 +799,9 @@
   </si>
   <si>
     <t>Calc_levy</t>
+  </si>
+  <si>
+    <t>NCD Years</t>
   </si>
 </sst>
 </file>
@@ -1659,37 +1659,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="109">
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="106">
     <dxf>
       <font>
         <color auto="1"/>
@@ -2755,8 +2725,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="108"/>
-      <tableStyleElement type="headerRow" dxfId="107"/>
+      <tableStyleElement type="wholeTable" dxfId="105"/>
+      <tableStyleElement type="headerRow" dxfId="104"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -2790,7 +2760,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3125,7 +3095,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3736,7 +3706,7 @@
         <v>5</v>
       </c>
       <c r="G4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
@@ -3782,7 +3752,7 @@
         <v>4</v>
       </c>
       <c r="G6" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
@@ -4049,7 +4019,7 @@
         <v>10</v>
       </c>
       <c r="G18" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
@@ -4060,16 +4030,16 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="D19">
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F19" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
@@ -4777,12 +4747,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B28:B34">
-    <cfRule type="expression" dxfId="106" priority="2">
+    <cfRule type="expression" dxfId="103" priority="2">
       <formula>EXACT(TEXT(B28,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:B27">
-    <cfRule type="expression" dxfId="105" priority="1">
+    <cfRule type="expression" dxfId="102" priority="1">
       <formula>EXACT(TEXT(B25,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4794,9 +4764,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K28" sqref="K28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4965,7 +4935,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -4989,7 +4959,7 @@
       </c>
       <c r="K4" s="3"/>
       <c r="L4" s="3" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="M4" s="3"/>
       <c r="N4" s="3"/>
@@ -5051,10 +5021,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="5" t="s">
@@ -5077,7 +5047,7 @@
       </c>
       <c r="K6" s="3"/>
       <c r="L6" s="5" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
@@ -5139,7 +5109,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
@@ -5163,7 +5133,7 @@
       </c>
       <c r="K8" s="3"/>
       <c r="L8" s="3" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="M8" s="3"/>
       <c r="N8" s="3"/>
@@ -5223,7 +5193,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C10" s="3"/>
       <c r="D10" s="3"/>
@@ -5247,7 +5217,7 @@
       </c>
       <c r="K10" s="3"/>
       <c r="L10" s="3" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="M10" s="3"/>
       <c r="N10" s="3"/>
@@ -5312,7 +5282,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C12" s="3"/>
       <c r="D12" s="3"/>
@@ -5336,7 +5306,7 @@
       </c>
       <c r="K12" s="3"/>
       <c r="L12" s="3" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="M12" s="3"/>
       <c r="N12" s="3" t="s">
@@ -5402,7 +5372,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
@@ -5426,7 +5396,7 @@
       </c>
       <c r="K14" s="3"/>
       <c r="L14" s="3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="M14" s="3"/>
       <c r="N14" s="3" t="s">
@@ -5492,7 +5462,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C16" s="3"/>
       <c r="D16" s="3"/>
@@ -5516,7 +5486,7 @@
       </c>
       <c r="K16" s="3"/>
       <c r="L16" s="3" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="M16" s="3"/>
       <c r="N16" s="3" t="s">
@@ -5582,7 +5552,7 @@
         <v>18</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -5606,7 +5576,7 @@
       </c>
       <c r="K18" s="3"/>
       <c r="L18" s="3" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="M18" s="3"/>
       <c r="N18" s="3" t="s">
@@ -5673,7 +5643,7 @@
         <v>20</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C20" s="3"/>
       <c r="D20" s="3"/>
@@ -5697,7 +5667,7 @@
       </c>
       <c r="K20" s="3"/>
       <c r="L20" s="3" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="M20" s="3"/>
       <c r="N20" s="3" t="s">
@@ -5764,7 +5734,7 @@
         <v>22</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C22" s="3"/>
       <c r="D22" s="3"/>
@@ -5788,7 +5758,7 @@
       </c>
       <c r="K22" s="3"/>
       <c r="L22" s="3" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="M22" s="3"/>
       <c r="N22" s="3" t="s">
@@ -5855,7 +5825,7 @@
         <v>24</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -5879,7 +5849,7 @@
       </c>
       <c r="K24" s="3"/>
       <c r="L24" s="5" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="M24" s="3"/>
       <c r="N24" s="3" t="s">
@@ -5927,7 +5897,7 @@
       </c>
       <c r="M25" s="3"/>
       <c r="N25" s="3" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="O25" s="3">
         <f>M50*1</f>
@@ -5943,7 +5913,7 @@
         <v>26</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -5967,7 +5937,7 @@
       </c>
       <c r="K26" s="3"/>
       <c r="L26" s="5" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="M26" s="3"/>
       <c r="N26" s="3" t="s">
@@ -6032,7 +6002,7 @@
         <v>28</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -6056,7 +6026,7 @@
       </c>
       <c r="K28" s="3"/>
       <c r="L28" s="3" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M28" s="3"/>
       <c r="N28" s="3" t="s">
@@ -6120,7 +6090,7 @@
         <v>30</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -6144,11 +6114,11 @@
       </c>
       <c r="K30" s="3"/>
       <c r="L30" s="3" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M30" s="3"/>
       <c r="N30" s="3" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="O30" s="3">
         <f>M50*1</f>
@@ -6193,7 +6163,7 @@
       </c>
       <c r="M31" s="3"/>
       <c r="N31" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="O31" s="3">
         <f>M50*1</f>
@@ -6247,7 +6217,7 @@
         <v>33</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -6271,7 +6241,7 @@
       </c>
       <c r="K33" s="3"/>
       <c r="L33" s="3" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="M33" s="3"/>
       <c r="N33" s="5"/>
@@ -6284,7 +6254,7 @@
         <v>34</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="3"/>
@@ -6308,7 +6278,7 @@
       </c>
       <c r="K34" s="3"/>
       <c r="L34" s="3" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="M34" s="8" t="s">
         <v>67</v>
@@ -6323,7 +6293,7 @@
         <v>35</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -6347,7 +6317,7 @@
       </c>
       <c r="K35" s="3"/>
       <c r="L35" s="3" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
@@ -6399,7 +6369,7 @@
         <v>37</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C37" s="3"/>
       <c r="D37" s="3"/>
@@ -6423,7 +6393,7 @@
       </c>
       <c r="K37" s="3"/>
       <c r="L37" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
@@ -6473,7 +6443,7 @@
         <v>39</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -6497,7 +6467,7 @@
       </c>
       <c r="K39" s="3"/>
       <c r="L39" s="5" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
@@ -6549,7 +6519,7 @@
         <v>41</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C41" s="3"/>
       <c r="D41" s="3"/>
@@ -6573,7 +6543,7 @@
       </c>
       <c r="K41" s="3"/>
       <c r="L41" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
@@ -6623,7 +6593,7 @@
         <v>43</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C43" s="3"/>
       <c r="D43" s="3"/>
@@ -6647,7 +6617,7 @@
       </c>
       <c r="K43" s="3"/>
       <c r="L43" s="5" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
@@ -6660,7 +6630,7 @@
         <v>44</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>223</v>
+        <v>257</v>
       </c>
       <c r="C44" s="3"/>
       <c r="D44" s="5"/>
@@ -6684,7 +6654,7 @@
       </c>
       <c r="K44" s="3"/>
       <c r="L44" s="5" t="s">
-        <v>223</v>
+        <v>257</v>
       </c>
       <c r="M44" s="3" t="s">
         <v>135</v>
@@ -6699,7 +6669,7 @@
         <v>45</v>
       </c>
       <c r="B45" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="C45" s="3"/>
       <c r="D45" s="3"/>
@@ -6723,7 +6693,7 @@
       </c>
       <c r="K45" s="3"/>
       <c r="L45" s="5" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
@@ -6775,7 +6745,7 @@
         <v>47</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
@@ -6799,7 +6769,7 @@
       </c>
       <c r="K47" s="3"/>
       <c r="L47" s="5" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="M47" s="3"/>
       <c r="N47" s="3"/>
@@ -6849,7 +6819,7 @@
         <v>49</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="5"/>
@@ -6873,7 +6843,7 @@
       </c>
       <c r="K49" s="3"/>
       <c r="L49" s="5" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="M49" s="8"/>
       <c r="N49" s="3"/>
@@ -6925,7 +6895,7 @@
         <v>51</v>
       </c>
       <c r="B51" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C51" s="3"/>
       <c r="D51" s="3"/>
@@ -6949,7 +6919,7 @@
       </c>
       <c r="K51" s="3"/>
       <c r="L51" s="3" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="M51" s="4"/>
       <c r="N51" s="3"/>
@@ -7001,7 +6971,7 @@
         <v>53</v>
       </c>
       <c r="B53" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C53" s="3"/>
       <c r="D53" s="3"/>
@@ -7025,7 +6995,7 @@
       </c>
       <c r="K53" s="3"/>
       <c r="L53" s="5" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="M53" s="3"/>
       <c r="N53" s="3"/>
@@ -7077,12 +7047,12 @@
         <v>55</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C55" s="3"/>
       <c r="D55" s="3"/>
       <c r="E55" s="3" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F55" s="3" t="s">
         <v>2</v>
@@ -7101,7 +7071,7 @@
       </c>
       <c r="K55" s="3"/>
       <c r="L55" s="3" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="M55" s="3"/>
       <c r="N55" s="3"/>
@@ -7114,462 +7084,462 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="V2:XFD7 S15:XFD15 S11:XFD11 AC1:XFD1 K1:Q1 N12:N24 Q11 Q15 P8:XFD10 Q12:XFD14 P12 P14 Q16:XFD25 O15:O24 P23:P24 P16:P17 P20:P21 O2:O12 P2:P7 A59:J1048576 L59:XFD1048576 L2 L3:M3 L5:M5 B6 E6:J6 B7:J7 L7:M7 B9:J9 L9:M9 B11:J11 L11:M11 B13:J13 L13:M13 B15:J15 L15:M15 E16 B17:J17 N26:XFD26 L17:M17 L19 B21:J21 L21:M21 B23:J23 L23:M23 B25:J25 L25:M25 B24 L24 B27:J27 L27:M27 B26 L26 B29:J29 L29:M29 L31:M31 B31:J32 L32 B34:J34 L34:M34 N33:XFD58 B36:J36 L36:M36 B38:J38 L38:M38 B40:J40 L40:M40 A3:A58 B42:J42 L42:M42 B44:J44 L44:M44 B46:J46 L46:M46 B48:J48 B49:D49 B50:J50 L48:M52 B52:J52 B51:D51 B54:J55 L54:M55 B3:J3 B5:J5 A1:J2 B19:J19 Q27:XFD32">
-    <cfRule type="expression" dxfId="104" priority="102">
+    <cfRule type="expression" dxfId="101" priority="102">
       <formula>EXACT(TEXT(A1,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M19">
-    <cfRule type="expression" dxfId="103" priority="100">
+    <cfRule type="expression" dxfId="100" priority="100">
       <formula>EXACT(TEXT(M19,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2">
-    <cfRule type="expression" dxfId="102" priority="98">
+    <cfRule type="expression" dxfId="99" priority="98">
       <formula>EXACT(TEXT(M2,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M32">
-    <cfRule type="expression" dxfId="101" priority="97">
+    <cfRule type="expression" dxfId="98" priority="97">
       <formula>EXACT(TEXT(M32,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P18">
-    <cfRule type="expression" dxfId="100" priority="94">
+    <cfRule type="expression" dxfId="97" priority="94">
       <formula>EXACT(TEXT(P18,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P25">
-    <cfRule type="expression" dxfId="99" priority="93">
+    <cfRule type="expression" dxfId="96" priority="93">
       <formula>EXACT(TEXT(P25,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N25:O25">
-    <cfRule type="expression" dxfId="98" priority="92">
+    <cfRule type="expression" dxfId="95" priority="92">
       <formula>EXACT(TEXT(N25,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6">
-    <cfRule type="expression" dxfId="97" priority="90">
+    <cfRule type="expression" dxfId="94" priority="90">
       <formula>EXACT(TEXT(L6,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8:J8">
-    <cfRule type="expression" dxfId="96" priority="89">
+    <cfRule type="expression" dxfId="93" priority="89">
       <formula>EXACT(TEXT(E8,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="expression" dxfId="95" priority="88">
+    <cfRule type="expression" dxfId="92" priority="88">
       <formula>EXACT(TEXT(B8,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8">
-    <cfRule type="expression" dxfId="94" priority="87">
+    <cfRule type="expression" dxfId="91" priority="87">
       <formula>EXACT(TEXT(L8,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="93" priority="86">
+    <cfRule type="expression" dxfId="90" priority="86">
       <formula>EXACT(TEXT(B10,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:J10">
-    <cfRule type="expression" dxfId="92" priority="85">
+    <cfRule type="expression" dxfId="89" priority="85">
       <formula>EXACT(TEXT(E10,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10">
-    <cfRule type="expression" dxfId="91" priority="84">
+    <cfRule type="expression" dxfId="88" priority="84">
       <formula>EXACT(TEXT(L10,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:J12">
-    <cfRule type="expression" dxfId="90" priority="83">
+    <cfRule type="expression" dxfId="87" priority="83">
       <formula>EXACT(TEXT(E12,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="89" priority="82">
+    <cfRule type="expression" dxfId="86" priority="82">
       <formula>EXACT(TEXT(B12,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L12">
-    <cfRule type="expression" dxfId="88" priority="81">
+    <cfRule type="expression" dxfId="85" priority="81">
       <formula>EXACT(TEXT(L12,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="87" priority="80">
+    <cfRule type="expression" dxfId="84" priority="80">
       <formula>EXACT(TEXT(B14,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:J14">
-    <cfRule type="expression" dxfId="86" priority="79">
+    <cfRule type="expression" dxfId="83" priority="79">
       <formula>EXACT(TEXT(E14,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14">
-    <cfRule type="expression" dxfId="85" priority="78">
+    <cfRule type="expression" dxfId="82" priority="78">
       <formula>EXACT(TEXT(L14,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="expression" dxfId="84" priority="77">
+    <cfRule type="expression" dxfId="81" priority="77">
       <formula>EXACT(TEXT(B16,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:J16">
-    <cfRule type="expression" dxfId="83" priority="76">
+    <cfRule type="expression" dxfId="80" priority="76">
       <formula>EXACT(TEXT(F16,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16">
-    <cfRule type="expression" dxfId="82" priority="75">
+    <cfRule type="expression" dxfId="79" priority="75">
       <formula>EXACT(TEXT(L16,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="expression" dxfId="81" priority="74">
+    <cfRule type="expression" dxfId="78" priority="74">
       <formula>EXACT(TEXT(B18,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18">
-    <cfRule type="expression" dxfId="80" priority="73">
+    <cfRule type="expression" dxfId="77" priority="73">
       <formula>EXACT(TEXT(E18,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18:J18">
-    <cfRule type="expression" dxfId="79" priority="72">
+    <cfRule type="expression" dxfId="76" priority="72">
       <formula>EXACT(TEXT(F18,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18">
-    <cfRule type="expression" dxfId="78" priority="71">
+    <cfRule type="expression" dxfId="75" priority="71">
       <formula>EXACT(TEXT(L18,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="expression" dxfId="77" priority="70">
+    <cfRule type="expression" dxfId="74" priority="70">
       <formula>EXACT(TEXT(B20,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="expression" dxfId="76" priority="69">
+    <cfRule type="expression" dxfId="73" priority="69">
       <formula>EXACT(TEXT(E20,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:J20">
-    <cfRule type="expression" dxfId="75" priority="68">
+    <cfRule type="expression" dxfId="72" priority="68">
       <formula>EXACT(TEXT(F20,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20">
-    <cfRule type="expression" dxfId="74" priority="66">
+    <cfRule type="expression" dxfId="71" priority="66">
       <formula>EXACT(TEXT(L20,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="expression" dxfId="73" priority="65">
+    <cfRule type="expression" dxfId="70" priority="65">
       <formula>EXACT(TEXT(B22,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="expression" dxfId="72" priority="64">
+    <cfRule type="expression" dxfId="69" priority="64">
       <formula>EXACT(TEXT(E22,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22:J22">
-    <cfRule type="expression" dxfId="71" priority="63">
+    <cfRule type="expression" dxfId="68" priority="63">
       <formula>EXACT(TEXT(F22,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22">
-    <cfRule type="expression" dxfId="70" priority="62">
+    <cfRule type="expression" dxfId="67" priority="62">
       <formula>EXACT(TEXT(L22,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="69" priority="61">
+    <cfRule type="expression" dxfId="66" priority="61">
       <formula>EXACT(TEXT(E24,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24:J24">
-    <cfRule type="expression" dxfId="68" priority="60">
+    <cfRule type="expression" dxfId="65" priority="60">
       <formula>EXACT(TEXT(F24,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="expression" dxfId="67" priority="59">
+    <cfRule type="expression" dxfId="64" priority="59">
       <formula>EXACT(TEXT(E26,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26:J26">
-    <cfRule type="expression" dxfId="66" priority="58">
+    <cfRule type="expression" dxfId="63" priority="58">
       <formula>EXACT(TEXT(F26,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="expression" dxfId="65" priority="57">
+    <cfRule type="expression" dxfId="62" priority="57">
       <formula>EXACT(TEXT(B28,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="expression" dxfId="64" priority="56">
+    <cfRule type="expression" dxfId="61" priority="56">
       <formula>EXACT(TEXT(E28,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28:J28">
-    <cfRule type="expression" dxfId="63" priority="55">
+    <cfRule type="expression" dxfId="60" priority="55">
       <formula>EXACT(TEXT(F28,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L28">
-    <cfRule type="expression" dxfId="62" priority="54">
+    <cfRule type="expression" dxfId="59" priority="54">
       <formula>EXACT(TEXT(L28,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="expression" dxfId="61" priority="53">
+    <cfRule type="expression" dxfId="58" priority="53">
       <formula>EXACT(TEXT(B30,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="expression" dxfId="60" priority="52">
+    <cfRule type="expression" dxfId="57" priority="52">
       <formula>EXACT(TEXT(E30,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30:J30">
-    <cfRule type="expression" dxfId="59" priority="51">
+    <cfRule type="expression" dxfId="56" priority="51">
       <formula>EXACT(TEXT(F30,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30">
-    <cfRule type="expression" dxfId="58" priority="50">
+    <cfRule type="expression" dxfId="55" priority="50">
       <formula>EXACT(TEXT(L30,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33">
-    <cfRule type="expression" dxfId="57" priority="49">
+    <cfRule type="expression" dxfId="54" priority="49">
       <formula>EXACT(TEXT(B33,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L33">
-    <cfRule type="expression" dxfId="56" priority="48">
+    <cfRule type="expression" dxfId="53" priority="48">
       <formula>EXACT(TEXT(L33,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="expression" dxfId="55" priority="47">
+    <cfRule type="expression" dxfId="52" priority="47">
       <formula>EXACT(TEXT(E33,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F33:J33">
-    <cfRule type="expression" dxfId="54" priority="46">
+    <cfRule type="expression" dxfId="51" priority="46">
       <formula>EXACT(TEXT(F33,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="expression" dxfId="53" priority="45">
+    <cfRule type="expression" dxfId="50" priority="45">
       <formula>EXACT(TEXT(B35,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="expression" dxfId="52" priority="44">
+    <cfRule type="expression" dxfId="49" priority="44">
       <formula>EXACT(TEXT(E35,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35:J35">
-    <cfRule type="expression" dxfId="51" priority="43">
+    <cfRule type="expression" dxfId="48" priority="43">
       <formula>EXACT(TEXT(F35,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L35">
-    <cfRule type="expression" dxfId="50" priority="42">
+    <cfRule type="expression" dxfId="47" priority="42">
       <formula>EXACT(TEXT(L35,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="expression" dxfId="49" priority="41">
+    <cfRule type="expression" dxfId="46" priority="41">
       <formula>EXACT(TEXT(B37,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="expression" dxfId="48" priority="40">
+    <cfRule type="expression" dxfId="45" priority="40">
       <formula>EXACT(TEXT(E37,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F37:J37">
-    <cfRule type="expression" dxfId="47" priority="39">
+    <cfRule type="expression" dxfId="44" priority="39">
       <formula>EXACT(TEXT(F37,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L37">
-    <cfRule type="expression" dxfId="46" priority="38">
+    <cfRule type="expression" dxfId="43" priority="38">
       <formula>EXACT(TEXT(L37,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="expression" dxfId="45" priority="37">
+    <cfRule type="expression" dxfId="42" priority="37">
       <formula>EXACT(TEXT(B39,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="expression" dxfId="44" priority="36">
+    <cfRule type="expression" dxfId="41" priority="36">
       <formula>EXACT(TEXT(E39,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F39:J39">
-    <cfRule type="expression" dxfId="43" priority="35">
+    <cfRule type="expression" dxfId="40" priority="35">
       <formula>EXACT(TEXT(F39,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L39">
-    <cfRule type="expression" dxfId="42" priority="34">
+    <cfRule type="expression" dxfId="39" priority="34">
       <formula>EXACT(TEXT(L39,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41">
-    <cfRule type="expression" dxfId="41" priority="33">
+    <cfRule type="expression" dxfId="38" priority="33">
       <formula>EXACT(TEXT(B41,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L41">
-    <cfRule type="expression" dxfId="40" priority="32">
+    <cfRule type="expression" dxfId="37" priority="32">
       <formula>EXACT(TEXT(L41,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="expression" dxfId="39" priority="31">
+    <cfRule type="expression" dxfId="36" priority="31">
       <formula>EXACT(TEXT(E41,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F41:J41">
-    <cfRule type="expression" dxfId="38" priority="30">
+    <cfRule type="expression" dxfId="35" priority="30">
       <formula>EXACT(TEXT(F41,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="expression" dxfId="37" priority="29">
+    <cfRule type="expression" dxfId="34" priority="29">
       <formula>EXACT(TEXT(B43,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="expression" dxfId="36" priority="28">
+    <cfRule type="expression" dxfId="33" priority="28">
       <formula>EXACT(TEXT(E43,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F43:J43">
-    <cfRule type="expression" dxfId="35" priority="27">
+    <cfRule type="expression" dxfId="32" priority="27">
       <formula>EXACT(TEXT(F43,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L43">
-    <cfRule type="expression" dxfId="34" priority="26">
+    <cfRule type="expression" dxfId="31" priority="26">
       <formula>EXACT(TEXT(L43,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="expression" dxfId="33" priority="25">
+    <cfRule type="expression" dxfId="30" priority="25">
       <formula>EXACT(TEXT(B45,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="expression" dxfId="32" priority="24">
+    <cfRule type="expression" dxfId="29" priority="24">
       <formula>EXACT(TEXT(E45,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45:J45">
-    <cfRule type="expression" dxfId="31" priority="23">
+    <cfRule type="expression" dxfId="28" priority="23">
       <formula>EXACT(TEXT(F45,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L45">
-    <cfRule type="expression" dxfId="30" priority="22">
+    <cfRule type="expression" dxfId="27" priority="22">
       <formula>EXACT(TEXT(L45,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="29" priority="21">
+    <cfRule type="expression" dxfId="26" priority="21">
       <formula>EXACT(TEXT(B47,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47">
-    <cfRule type="expression" dxfId="28" priority="20">
+    <cfRule type="expression" dxfId="25" priority="20">
       <formula>EXACT(TEXT(E47,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47:J47">
-    <cfRule type="expression" dxfId="27" priority="19">
+    <cfRule type="expression" dxfId="24" priority="19">
       <formula>EXACT(TEXT(F47,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L47">
-    <cfRule type="expression" dxfId="26" priority="18">
+    <cfRule type="expression" dxfId="23" priority="18">
       <formula>EXACT(TEXT(L47,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49">
-    <cfRule type="expression" dxfId="25" priority="17">
+    <cfRule type="expression" dxfId="22" priority="17">
       <formula>EXACT(TEXT(E49,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:J49">
-    <cfRule type="expression" dxfId="24" priority="16">
+    <cfRule type="expression" dxfId="21" priority="16">
       <formula>EXACT(TEXT(F49,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="expression" dxfId="23" priority="15">
+    <cfRule type="expression" dxfId="20" priority="15">
       <formula>EXACT(TEXT(E51,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F51:J51">
-    <cfRule type="expression" dxfId="22" priority="14">
+    <cfRule type="expression" dxfId="19" priority="14">
       <formula>EXACT(TEXT(F51,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="expression" dxfId="21" priority="13">
+    <cfRule type="expression" dxfId="18" priority="13">
       <formula>EXACT(TEXT(B53,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53">
-    <cfRule type="expression" dxfId="20" priority="12">
+    <cfRule type="expression" dxfId="17" priority="12">
       <formula>EXACT(TEXT(E53,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F53:J53">
-    <cfRule type="expression" dxfId="19" priority="11">
+    <cfRule type="expression" dxfId="16" priority="11">
       <formula>EXACT(TEXT(F53,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L53">
-    <cfRule type="expression" dxfId="18" priority="10">
+    <cfRule type="expression" dxfId="15" priority="10">
       <formula>EXACT(TEXT(L53,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N30:P30 N31 N32:P32 N28:O29">
-    <cfRule type="expression" dxfId="17" priority="5">
+    <cfRule type="expression" dxfId="14" priority="5">
       <formula>EXACT(TEXT(N28,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N27">
-    <cfRule type="expression" dxfId="16" priority="4">
+    <cfRule type="expression" dxfId="13" priority="4">
       <formula>EXACT(TEXT(N27,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P27">
-    <cfRule type="expression" dxfId="5" priority="3">
+    <cfRule type="expression" dxfId="12" priority="3">
       <formula>EXACT(TEXT(P27,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P28">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="11" priority="2">
       <formula>EXACT(TEXT(P28,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P29">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="10" priority="1">
       <formula>EXACT(TEXT(P29,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -7658,7 +7628,7 @@
         <v>14</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C1" s="15" t="s">
         <v>78</v>
@@ -9401,7 +9371,7 @@
         <v>14</v>
       </c>
       <c r="B138" s="48" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C138" s="49" t="s">
         <v>26</v>
@@ -10894,7 +10864,7 @@
         <v>14</v>
       </c>
       <c r="B246" s="57" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C246" s="56" t="s">
         <v>26</v>
@@ -13211,7 +13181,7 @@
     <mergeCell ref="A382:D382"/>
   </mergeCells>
   <conditionalFormatting sqref="B39">
-    <cfRule type="expression" dxfId="15" priority="1">
+    <cfRule type="expression" dxfId="9" priority="1">
       <formula>EXACT(TEXT(B39,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13262,7 +13232,7 @@
       </c>
       <c r="B3" s="38">
         <f ca="1">TODAY()</f>
-        <v>42866</v>
+        <v>42869</v>
       </c>
       <c r="C3" s="3">
         <f>IF(B$9&lt;B2,1,0)</f>
@@ -13275,7 +13245,7 @@
       </c>
       <c r="B4" s="38">
         <f ca="1">B3-1</f>
-        <v>42865</v>
+        <v>42868</v>
       </c>
       <c r="C4" s="3">
         <f ca="1">IF(B$9&lt;B3,1,0)</f>
@@ -13288,7 +13258,7 @@
       </c>
       <c r="B5" s="38">
         <f ca="1">EDATE(B3,-12)</f>
-        <v>42501</v>
+        <v>42504</v>
       </c>
       <c r="C5" s="3">
         <f ca="1">IF(B$9&lt;B5,1,0)</f>
@@ -13301,7 +13271,7 @@
       </c>
       <c r="B6" s="38">
         <f ca="1">EDATE(B3,-24)</f>
-        <v>42135</v>
+        <v>42138</v>
       </c>
       <c r="C6" s="3">
         <f ca="1">IF(B$9&lt;B6,1,0)</f>
@@ -13314,7 +13284,7 @@
       </c>
       <c r="B7" s="38">
         <f ca="1">EDATE(B3,-36)</f>
-        <v>41770</v>
+        <v>41773</v>
       </c>
       <c r="C7" s="3">
         <f ca="1">IF(B$9&lt;B7,1,0)</f>
@@ -13524,32 +13494,32 @@
     <mergeCell ref="A12:B12"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:B2 B5:B8 A4 B3 E17 C17 D5:D8 D10:D11 B10">
-    <cfRule type="expression" dxfId="14" priority="8">
+    <cfRule type="expression" dxfId="8" priority="8">
       <formula>EXACT(TEXT(A2,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A6">
-    <cfRule type="expression" dxfId="13" priority="5">
+    <cfRule type="expression" dxfId="7" priority="5">
       <formula>EXACT(TEXT(A6,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A7:A8 A16">
-    <cfRule type="expression" dxfId="12" priority="4">
+    <cfRule type="expression" dxfId="6" priority="4">
       <formula>EXACT(TEXT(A7,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B17">
-    <cfRule type="expression" dxfId="11" priority="3">
+    <cfRule type="expression" dxfId="5" priority="3">
       <formula>EXACT(TEXT(B17,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="expression" dxfId="10" priority="2">
+    <cfRule type="expression" dxfId="4" priority="2">
       <formula>EXACT(TEXT(A17,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A11:B11 A10">
-    <cfRule type="expression" dxfId="9" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>EXACT(TEXT(A10,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13980,17 +13950,17 @@
     <mergeCell ref="A14:B14"/>
   </mergeCells>
   <conditionalFormatting sqref="A2:B2 B5:B10 B3 D5:D12 D14:D15 B12">
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="2" priority="6">
       <formula>EXACT(TEXT(A2,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A10 A18">
-    <cfRule type="expression" dxfId="7" priority="4">
+    <cfRule type="expression" dxfId="1" priority="4">
       <formula>EXACT(TEXT(A10,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A12">
-    <cfRule type="expression" dxfId="6" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>EXACT(TEXT(A12,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Bug fix - Changes in master procedure for fuctions- mid result
</commit_message>
<xml_diff>
--- a/Authentication.WEB/ExcelConfig/config_file.xlsx
+++ b/Authentication.WEB/ExcelConfig/config_file.xlsx
@@ -2760,7 +2760,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000004000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3095,7 +3095,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -4764,9 +4764,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O21" sqref="O21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5543,7 +5543,7 @@
       </c>
       <c r="P17" s="3">
         <f>P16+O21</f>
-        <v>14692.1875</v>
+        <v>15192.1875</v>
       </c>
       <c r="Q17" s="3"/>
     </row>
@@ -5679,7 +5679,7 @@
       </c>
       <c r="P20" s="3">
         <f>P17*P19</f>
-        <v>14692.1875</v>
+        <v>15192.1875</v>
       </c>
       <c r="Q20" s="3"/>
     </row>
@@ -5721,11 +5721,12 @@
         <v>152</v>
       </c>
       <c r="O21" s="3">
-        <v>200</v>
+        <f>M21*100</f>
+        <v>700</v>
       </c>
       <c r="P21" s="3">
         <f>P20-O30</f>
-        <v>14691.9375</v>
+        <v>15191.9375</v>
       </c>
       <c r="Q21" s="3"/>
     </row>
@@ -5770,7 +5771,7 @@
       </c>
       <c r="P22" s="3">
         <f>P21*O25</f>
-        <v>3672.984375</v>
+        <v>3797.984375</v>
       </c>
       <c r="Q22" s="3"/>
     </row>
@@ -5816,7 +5817,7 @@
       </c>
       <c r="P23" s="3">
         <f>P21-P22</f>
-        <v>11018.953125</v>
+        <v>11393.953125</v>
       </c>
       <c r="Q23" s="3"/>
     </row>
@@ -5860,7 +5861,7 @@
       </c>
       <c r="P24" s="3">
         <f>P23*O26</f>
-        <v>3305.6859374999999</v>
+        <v>3418.1859374999999</v>
       </c>
       <c r="Q24" s="3"/>
     </row>
@@ -5949,7 +5950,7 @@
       </c>
       <c r="P26" s="3">
         <f>P23-P24</f>
-        <v>7713.2671874999996</v>
+        <v>7975.7671874999996</v>
       </c>
       <c r="Q26" s="3"/>
     </row>
@@ -5993,7 +5994,7 @@
       </c>
       <c r="P27" s="3">
         <f>P23-P24</f>
-        <v>7713.2671874999996</v>
+        <v>7975.7671874999996</v>
       </c>
       <c r="Q27" s="3"/>
     </row>
@@ -6037,7 +6038,7 @@
       </c>
       <c r="P28" s="3">
         <f>P23-P24</f>
-        <v>7713.2671874999996</v>
+        <v>7975.7671874999996</v>
       </c>
       <c r="Q28" s="3"/>
     </row>
@@ -6081,7 +6082,7 @@
       </c>
       <c r="P29" s="3">
         <f>P23-P24</f>
-        <v>7713.2671874999996</v>
+        <v>7975.7671874999996</v>
       </c>
       <c r="Q29" s="3"/>
     </row>
@@ -6126,7 +6127,7 @@
       </c>
       <c r="P30" s="3">
         <f>P26*1.01</f>
-        <v>7790.3998593749993</v>
+        <v>8055.5248593749993</v>
       </c>
       <c r="Q30" s="3"/>
     </row>
@@ -6171,7 +6172,7 @@
       </c>
       <c r="P31" s="3">
         <f>IF(M54="yes",P30,P26)</f>
-        <v>7790.3998593749993</v>
+        <v>8055.5248593749993</v>
       </c>
       <c r="Q31" s="3"/>
     </row>

</xml_diff>

<commit_message>
bug fix- add if else statement for input master procedure
</commit_message>
<xml_diff>
--- a/Authentication.WEB/ExcelConfig/config_file.xlsx
+++ b/Authentication.WEB/ExcelConfig/config_file.xlsx
@@ -1659,7 +1659,47 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="106">
+  <dxfs count="110">
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color auto="1"/>
@@ -2725,8 +2765,8 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
-      <tableStyleElement type="wholeTable" dxfId="105"/>
-      <tableStyleElement type="headerRow" dxfId="104"/>
+      <tableStyleElement type="wholeTable" dxfId="109"/>
+      <tableStyleElement type="headerRow" dxfId="108"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -4747,12 +4787,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B28:B34">
-    <cfRule type="expression" dxfId="103" priority="2">
+    <cfRule type="expression" dxfId="107" priority="2">
       <formula>EXACT(TEXT(B28,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:B27">
-    <cfRule type="expression" dxfId="102" priority="1">
+    <cfRule type="expression" dxfId="106" priority="1">
       <formula>EXACT(TEXT(B25,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4764,9 +4804,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O21" sqref="O21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F61" sqref="F61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5070,7 +5110,7 @@
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
       <c r="E7" s="3" t="s">
-        <v>9</v>
+        <v>88</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>2</v>
@@ -5785,7 +5825,7 @@
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3" t="s">
-        <v>13</v>
+        <v>86</v>
       </c>
       <c r="F23" s="3">
         <v>0</v>
@@ -6268,8 +6308,8 @@
       <c r="G34" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="H34" s="8" t="s">
-        <v>68</v>
+      <c r="H34" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="I34" s="3">
         <v>0</v>
@@ -6494,8 +6534,8 @@
       <c r="G40" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="H40" s="8" t="s">
-        <v>68</v>
+      <c r="H40" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="I40" s="3">
         <v>0</v>
@@ -6788,7 +6828,7 @@
       <c r="C48" s="3"/>
       <c r="D48" s="5"/>
       <c r="E48" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F48" s="8">
         <v>7</v>
@@ -6796,8 +6836,8 @@
       <c r="G48" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H48" s="8" t="s">
-        <v>68</v>
+      <c r="H48" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="I48" s="3">
         <v>0</v>
@@ -7014,7 +7054,7 @@
       <c r="C54" s="3"/>
       <c r="D54" s="5"/>
       <c r="E54" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F54" s="8">
         <v>7</v>
@@ -7022,8 +7062,8 @@
       <c r="G54" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H54" s="8" t="s">
-        <v>68</v>
+      <c r="H54" s="5" t="s">
+        <v>21</v>
       </c>
       <c r="I54" s="3">
         <v>0</v>
@@ -7084,468 +7124,488 @@
       <c r="A56" s="139"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="V2:XFD7 S15:XFD15 S11:XFD11 AC1:XFD1 K1:Q1 N12:N24 Q11 Q15 P8:XFD10 Q12:XFD14 P12 P14 Q16:XFD25 O15:O24 P23:P24 P16:P17 P20:P21 O2:O12 P2:P7 A59:J1048576 L59:XFD1048576 L2 L3:M3 L5:M5 B6 E6:J6 B7:J7 L7:M7 B9:J9 L9:M9 B11:J11 L11:M11 B13:J13 L13:M13 B15:J15 L15:M15 E16 B17:J17 N26:XFD26 L17:M17 L19 B21:J21 L21:M21 B23:J23 L23:M23 B25:J25 L25:M25 B24 L24 B27:J27 L27:M27 B26 L26 B29:J29 L29:M29 L31:M31 B31:J32 L32 B34:J34 L34:M34 N33:XFD58 B36:J36 L36:M36 B38:J38 L38:M38 B40:J40 L40:M40 A3:A58 B42:J42 L42:M42 B44:J44 L44:M44 B46:J46 L46:M46 B48:J48 B49:D49 B50:J50 L48:M52 B52:J52 B51:D51 B54:J55 L54:M55 B3:J3 B5:J5 A1:J2 B19:J19 Q27:XFD32">
-    <cfRule type="expression" dxfId="101" priority="102">
+  <conditionalFormatting sqref="V2:XFD7 S15:XFD15 S11:XFD11 AC1:XFD1 K1:Q1 N12:N24 Q11 Q15 P8:XFD10 Q12:XFD14 P12 P14 Q16:XFD25 O15:O24 P23:P24 P16:P17 P20:P21 O2:O12 P2:P7 A59:J1048576 L59:XFD1048576 L2 L3:M3 L5:M5 B6 E6:J6 B7:J7 L7:M7 B9:J9 L9:M9 B11:J11 L11:M11 B13:J13 L13:M13 B15:J15 L15:M15 E16 B17:J17 N26:XFD26 L17:M17 L19 B21:J21 L21:M21 B23:J23 L23:M23 B25:J25 L25:M25 B24 L24 B27:J27 L27:M27 B26 L26 B29:J29 L29:M29 L31:M31 B31:J32 L32 B34:G34 L34:M34 N33:XFD58 B36:J36 L36:M36 B38:J38 L38:M38 B40:G40 L40:M40 A3:A58 B42:J42 L42:M42 B44:J44 L44:M44 B46:J46 L46:M46 B48:G48 B49:D49 B50:J50 L48:M52 B52:J52 B51:D51 B55:J55 L54:M55 B3:J3 B5:J5 A1:J2 B19:J19 Q27:XFD32 B54:G54 I54:J54 I48:J48 I40:J40 I34:J34">
+    <cfRule type="expression" dxfId="105" priority="106">
       <formula>EXACT(TEXT(A1,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M19">
-    <cfRule type="expression" dxfId="100" priority="100">
+    <cfRule type="expression" dxfId="104" priority="104">
       <formula>EXACT(TEXT(M19,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2">
-    <cfRule type="expression" dxfId="99" priority="98">
+    <cfRule type="expression" dxfId="103" priority="102">
       <formula>EXACT(TEXT(M2,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M32">
-    <cfRule type="expression" dxfId="98" priority="97">
+    <cfRule type="expression" dxfId="102" priority="101">
       <formula>EXACT(TEXT(M32,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P18">
-    <cfRule type="expression" dxfId="97" priority="94">
+    <cfRule type="expression" dxfId="101" priority="98">
       <formula>EXACT(TEXT(P18,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P25">
-    <cfRule type="expression" dxfId="96" priority="93">
+    <cfRule type="expression" dxfId="100" priority="97">
       <formula>EXACT(TEXT(P25,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N25:O25">
-    <cfRule type="expression" dxfId="95" priority="92">
+    <cfRule type="expression" dxfId="99" priority="96">
       <formula>EXACT(TEXT(N25,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L6">
-    <cfRule type="expression" dxfId="94" priority="90">
+    <cfRule type="expression" dxfId="98" priority="94">
       <formula>EXACT(TEXT(L6,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8:J8">
-    <cfRule type="expression" dxfId="93" priority="89">
+    <cfRule type="expression" dxfId="97" priority="93">
       <formula>EXACT(TEXT(E8,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B8">
-    <cfRule type="expression" dxfId="92" priority="88">
+    <cfRule type="expression" dxfId="96" priority="92">
       <formula>EXACT(TEXT(B8,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L8">
-    <cfRule type="expression" dxfId="91" priority="87">
+    <cfRule type="expression" dxfId="95" priority="91">
       <formula>EXACT(TEXT(L8,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B10">
-    <cfRule type="expression" dxfId="90" priority="86">
+    <cfRule type="expression" dxfId="94" priority="90">
       <formula>EXACT(TEXT(B10,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10:J10">
-    <cfRule type="expression" dxfId="89" priority="85">
+    <cfRule type="expression" dxfId="93" priority="89">
       <formula>EXACT(TEXT(E10,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L10">
-    <cfRule type="expression" dxfId="88" priority="84">
+    <cfRule type="expression" dxfId="92" priority="88">
       <formula>EXACT(TEXT(L10,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12:J12">
-    <cfRule type="expression" dxfId="87" priority="83">
+    <cfRule type="expression" dxfId="91" priority="87">
       <formula>EXACT(TEXT(E12,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B12">
-    <cfRule type="expression" dxfId="86" priority="82">
+    <cfRule type="expression" dxfId="90" priority="86">
       <formula>EXACT(TEXT(B12,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L12">
-    <cfRule type="expression" dxfId="85" priority="81">
+    <cfRule type="expression" dxfId="89" priority="85">
       <formula>EXACT(TEXT(L12,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B14">
-    <cfRule type="expression" dxfId="84" priority="80">
+    <cfRule type="expression" dxfId="88" priority="84">
       <formula>EXACT(TEXT(B14,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14:J14">
-    <cfRule type="expression" dxfId="83" priority="79">
+    <cfRule type="expression" dxfId="87" priority="83">
       <formula>EXACT(TEXT(E14,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L14">
-    <cfRule type="expression" dxfId="82" priority="78">
+    <cfRule type="expression" dxfId="86" priority="82">
       <formula>EXACT(TEXT(L14,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B16">
-    <cfRule type="expression" dxfId="81" priority="77">
+    <cfRule type="expression" dxfId="85" priority="81">
       <formula>EXACT(TEXT(B16,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F16:J16">
-    <cfRule type="expression" dxfId="80" priority="76">
+    <cfRule type="expression" dxfId="84" priority="80">
       <formula>EXACT(TEXT(F16,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L16">
-    <cfRule type="expression" dxfId="79" priority="75">
+    <cfRule type="expression" dxfId="83" priority="79">
       <formula>EXACT(TEXT(L16,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B18">
-    <cfRule type="expression" dxfId="78" priority="74">
+    <cfRule type="expression" dxfId="82" priority="78">
       <formula>EXACT(TEXT(B18,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E18">
-    <cfRule type="expression" dxfId="77" priority="73">
+    <cfRule type="expression" dxfId="81" priority="77">
       <formula>EXACT(TEXT(E18,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18:J18">
-    <cfRule type="expression" dxfId="76" priority="72">
+    <cfRule type="expression" dxfId="80" priority="76">
       <formula>EXACT(TEXT(F18,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18">
-    <cfRule type="expression" dxfId="75" priority="71">
+    <cfRule type="expression" dxfId="79" priority="75">
       <formula>EXACT(TEXT(L18,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B20">
-    <cfRule type="expression" dxfId="74" priority="70">
+    <cfRule type="expression" dxfId="78" priority="74">
       <formula>EXACT(TEXT(B20,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20">
-    <cfRule type="expression" dxfId="73" priority="69">
+    <cfRule type="expression" dxfId="77" priority="73">
       <formula>EXACT(TEXT(E20,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F20:J20">
-    <cfRule type="expression" dxfId="72" priority="68">
+    <cfRule type="expression" dxfId="76" priority="72">
       <formula>EXACT(TEXT(F20,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L20">
-    <cfRule type="expression" dxfId="71" priority="66">
+    <cfRule type="expression" dxfId="75" priority="70">
       <formula>EXACT(TEXT(L20,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B22">
-    <cfRule type="expression" dxfId="70" priority="65">
+    <cfRule type="expression" dxfId="74" priority="69">
       <formula>EXACT(TEXT(B22,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E22">
-    <cfRule type="expression" dxfId="69" priority="64">
+    <cfRule type="expression" dxfId="73" priority="68">
       <formula>EXACT(TEXT(E22,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F22:J22">
-    <cfRule type="expression" dxfId="68" priority="63">
+    <cfRule type="expression" dxfId="72" priority="67">
       <formula>EXACT(TEXT(F22,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L22">
-    <cfRule type="expression" dxfId="67" priority="62">
+    <cfRule type="expression" dxfId="71" priority="66">
       <formula>EXACT(TEXT(L22,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E24">
-    <cfRule type="expression" dxfId="66" priority="61">
+    <cfRule type="expression" dxfId="70" priority="65">
       <formula>EXACT(TEXT(E24,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F24:J24">
-    <cfRule type="expression" dxfId="65" priority="60">
+    <cfRule type="expression" dxfId="69" priority="64">
       <formula>EXACT(TEXT(F24,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E26">
-    <cfRule type="expression" dxfId="64" priority="59">
+    <cfRule type="expression" dxfId="68" priority="63">
       <formula>EXACT(TEXT(E26,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26:J26">
-    <cfRule type="expression" dxfId="63" priority="58">
+    <cfRule type="expression" dxfId="67" priority="62">
       <formula>EXACT(TEXT(F26,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B28">
-    <cfRule type="expression" dxfId="62" priority="57">
+    <cfRule type="expression" dxfId="66" priority="61">
       <formula>EXACT(TEXT(B28,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E28">
-    <cfRule type="expression" dxfId="61" priority="56">
+    <cfRule type="expression" dxfId="65" priority="60">
       <formula>EXACT(TEXT(E28,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28:J28">
-    <cfRule type="expression" dxfId="60" priority="55">
+    <cfRule type="expression" dxfId="64" priority="59">
       <formula>EXACT(TEXT(F28,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L28">
-    <cfRule type="expression" dxfId="59" priority="54">
+    <cfRule type="expression" dxfId="63" priority="58">
       <formula>EXACT(TEXT(L28,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B30">
-    <cfRule type="expression" dxfId="58" priority="53">
+    <cfRule type="expression" dxfId="62" priority="57">
       <formula>EXACT(TEXT(B30,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E30">
-    <cfRule type="expression" dxfId="57" priority="52">
+    <cfRule type="expression" dxfId="61" priority="56">
       <formula>EXACT(TEXT(E30,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F30:J30">
-    <cfRule type="expression" dxfId="56" priority="51">
+    <cfRule type="expression" dxfId="60" priority="55">
       <formula>EXACT(TEXT(F30,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30">
-    <cfRule type="expression" dxfId="55" priority="50">
+    <cfRule type="expression" dxfId="59" priority="54">
       <formula>EXACT(TEXT(L30,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B33">
-    <cfRule type="expression" dxfId="54" priority="49">
+    <cfRule type="expression" dxfId="58" priority="53">
       <formula>EXACT(TEXT(B33,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L33">
-    <cfRule type="expression" dxfId="53" priority="48">
+    <cfRule type="expression" dxfId="57" priority="52">
       <formula>EXACT(TEXT(L33,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E33">
-    <cfRule type="expression" dxfId="52" priority="47">
+    <cfRule type="expression" dxfId="56" priority="51">
       <formula>EXACT(TEXT(E33,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F33:J33">
-    <cfRule type="expression" dxfId="51" priority="46">
+    <cfRule type="expression" dxfId="55" priority="50">
       <formula>EXACT(TEXT(F33,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B35">
-    <cfRule type="expression" dxfId="50" priority="45">
+    <cfRule type="expression" dxfId="54" priority="49">
       <formula>EXACT(TEXT(B35,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E35">
-    <cfRule type="expression" dxfId="49" priority="44">
+    <cfRule type="expression" dxfId="53" priority="48">
       <formula>EXACT(TEXT(E35,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35:J35">
-    <cfRule type="expression" dxfId="48" priority="43">
+    <cfRule type="expression" dxfId="52" priority="47">
       <formula>EXACT(TEXT(F35,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L35">
-    <cfRule type="expression" dxfId="47" priority="42">
+    <cfRule type="expression" dxfId="51" priority="46">
       <formula>EXACT(TEXT(L35,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B37">
-    <cfRule type="expression" dxfId="46" priority="41">
+    <cfRule type="expression" dxfId="50" priority="45">
       <formula>EXACT(TEXT(B37,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E37">
-    <cfRule type="expression" dxfId="45" priority="40">
+    <cfRule type="expression" dxfId="49" priority="44">
       <formula>EXACT(TEXT(E37,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F37:J37">
-    <cfRule type="expression" dxfId="44" priority="39">
+    <cfRule type="expression" dxfId="48" priority="43">
       <formula>EXACT(TEXT(F37,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L37">
-    <cfRule type="expression" dxfId="43" priority="38">
+    <cfRule type="expression" dxfId="47" priority="42">
       <formula>EXACT(TEXT(L37,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B39">
-    <cfRule type="expression" dxfId="42" priority="37">
+    <cfRule type="expression" dxfId="46" priority="41">
       <formula>EXACT(TEXT(B39,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E39">
-    <cfRule type="expression" dxfId="41" priority="36">
+    <cfRule type="expression" dxfId="45" priority="40">
       <formula>EXACT(TEXT(E39,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F39:J39">
-    <cfRule type="expression" dxfId="40" priority="35">
+    <cfRule type="expression" dxfId="44" priority="39">
       <formula>EXACT(TEXT(F39,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L39">
-    <cfRule type="expression" dxfId="39" priority="34">
+    <cfRule type="expression" dxfId="43" priority="38">
       <formula>EXACT(TEXT(L39,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B41">
-    <cfRule type="expression" dxfId="38" priority="33">
+    <cfRule type="expression" dxfId="42" priority="37">
       <formula>EXACT(TEXT(B41,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L41">
-    <cfRule type="expression" dxfId="37" priority="32">
+    <cfRule type="expression" dxfId="41" priority="36">
       <formula>EXACT(TEXT(L41,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E41">
-    <cfRule type="expression" dxfId="36" priority="31">
+    <cfRule type="expression" dxfId="40" priority="35">
       <formula>EXACT(TEXT(E41,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F41:J41">
-    <cfRule type="expression" dxfId="35" priority="30">
+    <cfRule type="expression" dxfId="39" priority="34">
       <formula>EXACT(TEXT(F41,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B43">
-    <cfRule type="expression" dxfId="34" priority="29">
+    <cfRule type="expression" dxfId="38" priority="33">
       <formula>EXACT(TEXT(B43,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E43">
-    <cfRule type="expression" dxfId="33" priority="28">
+    <cfRule type="expression" dxfId="37" priority="32">
       <formula>EXACT(TEXT(E43,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F43:J43">
-    <cfRule type="expression" dxfId="32" priority="27">
+    <cfRule type="expression" dxfId="36" priority="31">
       <formula>EXACT(TEXT(F43,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L43">
-    <cfRule type="expression" dxfId="31" priority="26">
+    <cfRule type="expression" dxfId="35" priority="30">
       <formula>EXACT(TEXT(L43,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B45">
-    <cfRule type="expression" dxfId="30" priority="25">
+    <cfRule type="expression" dxfId="34" priority="29">
       <formula>EXACT(TEXT(B45,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E45">
-    <cfRule type="expression" dxfId="29" priority="24">
+    <cfRule type="expression" dxfId="33" priority="28">
       <formula>EXACT(TEXT(E45,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F45:J45">
-    <cfRule type="expression" dxfId="28" priority="23">
+    <cfRule type="expression" dxfId="32" priority="27">
       <formula>EXACT(TEXT(F45,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L45">
-    <cfRule type="expression" dxfId="27" priority="22">
+    <cfRule type="expression" dxfId="31" priority="26">
       <formula>EXACT(TEXT(L45,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B47">
-    <cfRule type="expression" dxfId="26" priority="21">
+    <cfRule type="expression" dxfId="30" priority="25">
       <formula>EXACT(TEXT(B47,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E47">
-    <cfRule type="expression" dxfId="25" priority="20">
+    <cfRule type="expression" dxfId="29" priority="24">
       <formula>EXACT(TEXT(E47,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F47:J47">
-    <cfRule type="expression" dxfId="24" priority="19">
+    <cfRule type="expression" dxfId="28" priority="23">
       <formula>EXACT(TEXT(F47,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L47">
-    <cfRule type="expression" dxfId="23" priority="18">
+    <cfRule type="expression" dxfId="27" priority="22">
       <formula>EXACT(TEXT(L47,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E49">
-    <cfRule type="expression" dxfId="22" priority="17">
+    <cfRule type="expression" dxfId="26" priority="21">
       <formula>EXACT(TEXT(E49,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F49:J49">
-    <cfRule type="expression" dxfId="21" priority="16">
+    <cfRule type="expression" dxfId="25" priority="20">
       <formula>EXACT(TEXT(F49,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E51">
-    <cfRule type="expression" dxfId="20" priority="15">
+    <cfRule type="expression" dxfId="24" priority="19">
       <formula>EXACT(TEXT(E51,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F51:J51">
-    <cfRule type="expression" dxfId="19" priority="14">
+    <cfRule type="expression" dxfId="23" priority="18">
       <formula>EXACT(TEXT(F51,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B53">
-    <cfRule type="expression" dxfId="18" priority="13">
+    <cfRule type="expression" dxfId="22" priority="17">
       <formula>EXACT(TEXT(B53,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E53">
-    <cfRule type="expression" dxfId="17" priority="12">
+    <cfRule type="expression" dxfId="21" priority="16">
       <formula>EXACT(TEXT(E53,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F53:J53">
-    <cfRule type="expression" dxfId="16" priority="11">
+    <cfRule type="expression" dxfId="20" priority="15">
       <formula>EXACT(TEXT(F53,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L53">
-    <cfRule type="expression" dxfId="15" priority="10">
+    <cfRule type="expression" dxfId="19" priority="14">
       <formula>EXACT(TEXT(L53,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N30:P30 N31 N32:P32 N28:O29">
-    <cfRule type="expression" dxfId="14" priority="5">
+    <cfRule type="expression" dxfId="18" priority="9">
       <formula>EXACT(TEXT(N28,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N27">
-    <cfRule type="expression" dxfId="13" priority="4">
+    <cfRule type="expression" dxfId="17" priority="8">
       <formula>EXACT(TEXT(N27,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P27">
-    <cfRule type="expression" dxfId="12" priority="3">
+    <cfRule type="expression" dxfId="16" priority="7">
       <formula>EXACT(TEXT(P27,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P28">
-    <cfRule type="expression" dxfId="11" priority="2">
+    <cfRule type="expression" dxfId="15" priority="6">
       <formula>EXACT(TEXT(P28,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P29">
-    <cfRule type="expression" dxfId="10" priority="1">
+    <cfRule type="expression" dxfId="14" priority="5">
       <formula>EXACT(TEXT(P29,"text"),"?")</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="H54">
+    <cfRule type="expression" dxfId="13" priority="4">
+      <formula>EXACT(TEXT(H54,"text"),"?")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H48">
+    <cfRule type="expression" dxfId="12" priority="3">
+      <formula>EXACT(TEXT(H48,"text"),"?")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H40">
+    <cfRule type="expression" dxfId="11" priority="2">
+      <formula>EXACT(TEXT(H40,"text"),"?")</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H34">
+    <cfRule type="expression" dxfId="10" priority="1">
+      <formula>EXACT(TEXT(H34,"text"),"?")</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H48 H54 H40 M46 M50">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M46 M50">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -7582,7 +7642,7 @@
           <x14:formula1>
             <xm:f>Lists!$C$30:$C$31</xm:f>
           </x14:formula1>
-          <xm:sqref>M54 M34 M36 H34 H36 M40 M49</xm:sqref>
+          <xm:sqref>M54 M34 M36 M49 H36 M40</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>

</xml_diff>